<commit_message>
Updated BOM to replace L9-10 by 0 Ohm resistors
</commit_message>
<xml_diff>
--- a/FPGA1394V3-BOM.xlsx
+++ b/FPGA1394V3-BOM.xlsx
@@ -10,14 +10,14 @@
     <sheet name="FPGA Rev 3" sheetId="42" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'FPGA Rev 3'!$A$4:$J$92</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'FPGA Rev 3'!$A$4:$J$93</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="421">
   <si>
     <t>Do Not Install</t>
   </si>
@@ -1231,9 +1231,6 @@
     <t xml:space="preserve">L6-7 </t>
   </si>
   <si>
-    <t xml:space="preserve">L8-10 </t>
-  </si>
-  <si>
     <t xml:space="preserve">L11-14 </t>
   </si>
   <si>
@@ -1485,6 +1482,21 @@
   </si>
   <si>
     <t>IC, Crystal Oscillator, 25.00MHz</t>
+  </si>
+  <si>
+    <t>L9-10</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>RES, 0</t>
+  </si>
+  <si>
+    <t>2, 5</t>
+  </si>
+  <si>
+    <t>L9-10 have been replaced by 0 Ohm resistors</t>
   </si>
 </sst>
 </file>
@@ -1895,32 +1907,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2229,7 +2241,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M108"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -2255,7 +2267,7 @@
     <row r="1" spans="1:13" ht="29.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2285,7 +2297,7 @@
     <row r="3" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="22">
-        <v>44818</v>
+        <v>45050</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2367,7 +2379,7 @@
       <c r="L6" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="88" t="s">
+      <c r="M6" s="84" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2398,11 +2410,11 @@
       <c r="J7" s="58"/>
       <c r="K7" s="51"/>
       <c r="L7" s="11"/>
-      <c r="M7" s="89"/>
+      <c r="M7" s="85"/>
     </row>
     <row r="8" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
-        <f t="shared" ref="A8:A72" si="0">A7+1</f>
+        <f t="shared" ref="A8:A73" si="0">A7+1</f>
         <v>2</v>
       </c>
       <c r="B8" s="25">
@@ -2438,7 +2450,7 @@
       <c r="L8" s="19">
         <v>2.4E-2</v>
       </c>
-      <c r="M8" s="89">
+      <c r="M8" s="85">
         <f>B8*L8</f>
         <v>4.8000000000000001E-2</v>
       </c>
@@ -2471,7 +2483,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="50"/>
       <c r="L9" s="19"/>
-      <c r="M9" s="89"/>
+      <c r="M9" s="85"/>
     </row>
     <row r="10" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
@@ -2503,7 +2515,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="50"/>
       <c r="L10" s="19"/>
-      <c r="M10" s="89"/>
+      <c r="M10" s="85"/>
     </row>
     <row r="11" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
@@ -2537,7 +2549,7 @@
       </c>
       <c r="K11" s="50"/>
       <c r="L11" s="19"/>
-      <c r="M11" s="89"/>
+      <c r="M11" s="85"/>
     </row>
     <row r="12" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
@@ -2573,7 +2585,7 @@
       <c r="L12" s="77">
         <v>0.13611999999999999</v>
       </c>
-      <c r="M12" s="89">
+      <c r="M12" s="85">
         <f t="shared" ref="M12:M21" si="1">B12*L12</f>
         <v>0.68059999999999998</v>
       </c>
@@ -2612,7 +2624,7 @@
       <c r="L13" s="19">
         <v>0.43258999999999997</v>
       </c>
-      <c r="M13" s="89">
+      <c r="M13" s="85">
         <f t="shared" si="1"/>
         <v>5.6236699999999997</v>
       </c>
@@ -2651,7 +2663,7 @@
       <c r="L14" s="77">
         <v>0.59299999999999997</v>
       </c>
-      <c r="M14" s="89">
+      <c r="M14" s="85">
         <f t="shared" si="1"/>
         <v>1.1859999999999999</v>
       </c>
@@ -2694,7 +2706,7 @@
       <c r="L15" s="11">
         <v>0.64890000000000003</v>
       </c>
-      <c r="M15" s="89">
+      <c r="M15" s="85">
         <f t="shared" si="1"/>
         <v>3.2445000000000004</v>
       </c>
@@ -2737,7 +2749,7 @@
       <c r="L16" s="11">
         <v>1.2175</v>
       </c>
-      <c r="M16" s="89">
+      <c r="M16" s="85">
         <f t="shared" si="1"/>
         <v>2.4350000000000001</v>
       </c>
@@ -2780,7 +2792,7 @@
       <c r="L17" s="11">
         <v>4.8</v>
       </c>
-      <c r="M17" s="89">
+      <c r="M17" s="85">
         <f t="shared" si="1"/>
         <v>9.6</v>
       </c>
@@ -2823,7 +2835,7 @@
       <c r="L18" s="19">
         <v>3.2381700000000002</v>
       </c>
-      <c r="M18" s="89">
+      <c r="M18" s="85">
         <f t="shared" si="1"/>
         <v>6.4763400000000004</v>
       </c>
@@ -2866,7 +2878,7 @@
       <c r="L19" s="11">
         <v>1.35</v>
       </c>
-      <c r="M19" s="89">
+      <c r="M19" s="85">
         <f t="shared" si="1"/>
         <v>2.7</v>
       </c>
@@ -2909,7 +2921,7 @@
       <c r="L20" s="19">
         <v>1.3098000000000001</v>
       </c>
-      <c r="M20" s="89">
+      <c r="M20" s="85">
         <f t="shared" si="1"/>
         <v>1.3098000000000001</v>
       </c>
@@ -2948,7 +2960,7 @@
       <c r="L21" s="77">
         <v>2.3774600000000001</v>
       </c>
-      <c r="M21" s="89">
+      <c r="M21" s="85">
         <f t="shared" si="1"/>
         <v>4.7549200000000003</v>
       </c>
@@ -2985,7 +2997,7 @@
       </c>
       <c r="K22" s="50"/>
       <c r="L22" s="19"/>
-      <c r="M22" s="89"/>
+      <c r="M22" s="85"/>
     </row>
     <row r="23" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
@@ -3019,7 +3031,7 @@
       </c>
       <c r="K23" s="50"/>
       <c r="L23" s="19"/>
-      <c r="M23" s="89"/>
+      <c r="M23" s="85"/>
     </row>
     <row r="24" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
@@ -3053,7 +3065,7 @@
       <c r="L24" s="19">
         <v>7.2650000000000006E-2</v>
       </c>
-      <c r="M24" s="89">
+      <c r="M24" s="85">
         <f t="shared" ref="M24:M31" si="2">B24*L24</f>
         <v>1.8162500000000001</v>
       </c>
@@ -3090,7 +3102,7 @@
       <c r="L25" s="19">
         <v>0.41160000000000002</v>
       </c>
-      <c r="M25" s="89">
+      <c r="M25" s="85">
         <f t="shared" si="2"/>
         <v>0.41160000000000002</v>
       </c>
@@ -3133,7 +3145,7 @@
       <c r="L26" s="77">
         <v>0.31574999999999998</v>
       </c>
-      <c r="M26" s="89">
+      <c r="M26" s="85">
         <f t="shared" si="2"/>
         <v>0.94724999999999993</v>
       </c>
@@ -3176,7 +3188,7 @@
       <c r="L27" s="19">
         <v>4.31034482758621E-2</v>
       </c>
-      <c r="M27" s="89">
+      <c r="M27" s="85">
         <f t="shared" si="2"/>
         <v>0.3448275862068968</v>
       </c>
@@ -3219,7 +3231,7 @@
       <c r="L28" s="11">
         <v>5.72</v>
       </c>
-      <c r="M28" s="89">
+      <c r="M28" s="85">
         <f t="shared" si="2"/>
         <v>11.44</v>
       </c>
@@ -3245,7 +3257,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H29" s="14" t="s">
         <v>15</v>
@@ -3262,7 +3274,7 @@
       <c r="L29" s="19">
         <v>3.3448000000000002</v>
       </c>
-      <c r="M29" s="89">
+      <c r="M29" s="85">
         <f t="shared" si="2"/>
         <v>6.6896000000000004</v>
       </c>
@@ -3301,7 +3313,7 @@
       <c r="L30" s="77">
         <v>2.1168</v>
       </c>
-      <c r="M30" s="89">
+      <c r="M30" s="85">
         <f t="shared" si="2"/>
         <v>2.1168</v>
       </c>
@@ -3321,7 +3333,7 @@
         <v>22</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>1</v>
@@ -3344,7 +3356,7 @@
       <c r="L31" s="19">
         <v>0.09</v>
       </c>
-      <c r="M31" s="89">
+      <c r="M31" s="85">
         <f t="shared" si="2"/>
         <v>0.09</v>
       </c>
@@ -3361,31 +3373,31 @@
         <v>312</v>
       </c>
       <c r="D32" s="55" t="s">
+        <v>377</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="F32" s="20" t="s">
         <v>378</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="F32" s="20" t="s">
+      <c r="G32" s="13">
+        <v>2</v>
+      </c>
+      <c r="H32" s="51" t="s">
         <v>379</v>
-      </c>
-      <c r="G32" s="13">
-        <v>2</v>
-      </c>
-      <c r="H32" s="51" t="s">
-        <v>380</v>
       </c>
       <c r="I32" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="J32" s="84" t="s">
+      <c r="J32" s="80" t="s">
+        <v>380</v>
+      </c>
+      <c r="K32" s="51" t="s">
         <v>381</v>
       </c>
-      <c r="K32" s="51" t="s">
-        <v>382</v>
-      </c>
       <c r="L32" s="19"/>
-      <c r="M32" s="89"/>
+      <c r="M32" s="85"/>
     </row>
     <row r="33" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
@@ -3399,30 +3411,30 @@
         <v>343</v>
       </c>
       <c r="D33" s="66" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E33" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="85" t="s">
+      <c r="F33" s="81" t="s">
+        <v>382</v>
+      </c>
+      <c r="G33" s="37"/>
+      <c r="H33" s="80" t="s">
         <v>383</v>
-      </c>
-      <c r="G33" s="37"/>
-      <c r="H33" s="84" t="s">
-        <v>384</v>
       </c>
       <c r="I33" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J33" s="66" t="s">
-        <v>385</v>
-      </c>
-      <c r="K33" s="84"/>
-      <c r="L33" s="86">
+        <v>384</v>
+      </c>
+      <c r="K33" s="80"/>
+      <c r="L33" s="82">
         <v>11.4</v>
       </c>
-      <c r="M33" s="89">
-        <f t="shared" ref="M33:M47" si="3">B33*L33</f>
+      <c r="M33" s="85">
+        <f t="shared" ref="M33:M48" si="3">B33*L33</f>
         <v>11.4</v>
       </c>
     </row>
@@ -3438,29 +3450,29 @@
         <v>344</v>
       </c>
       <c r="D34" s="66" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E34" s="66" t="s">
+        <v>388</v>
+      </c>
+      <c r="F34" s="81" t="s">
+        <v>387</v>
+      </c>
+      <c r="G34" s="37"/>
+      <c r="H34" s="80" t="s">
         <v>389</v>
-      </c>
-      <c r="F34" s="85" t="s">
-        <v>388</v>
-      </c>
-      <c r="G34" s="37"/>
-      <c r="H34" s="84" t="s">
-        <v>390</v>
       </c>
       <c r="I34" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J34" s="66" t="s">
-        <v>387</v>
-      </c>
-      <c r="K34" s="84"/>
-      <c r="L34" s="86">
+        <v>386</v>
+      </c>
+      <c r="K34" s="80"/>
+      <c r="L34" s="82">
         <v>0.43</v>
       </c>
-      <c r="M34" s="89">
+      <c r="M34" s="85">
         <f t="shared" si="3"/>
         <v>0.43</v>
       </c>
@@ -3477,31 +3489,31 @@
         <v>313</v>
       </c>
       <c r="D35" s="66" t="s">
+        <v>398</v>
+      </c>
+      <c r="E35" s="66" t="s">
         <v>399</v>
       </c>
-      <c r="E35" s="66" t="s">
-        <v>400</v>
-      </c>
-      <c r="F35" s="85" t="s">
-        <v>397</v>
+      <c r="F35" s="81" t="s">
+        <v>396</v>
       </c>
       <c r="G35" s="13">
         <v>2</v>
       </c>
-      <c r="H35" s="84" t="s">
-        <v>396</v>
+      <c r="H35" s="80" t="s">
+        <v>395</v>
       </c>
       <c r="I35" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J35" s="66" t="s">
-        <v>395</v>
-      </c>
-      <c r="K35" s="84" t="s">
-        <v>398</v>
-      </c>
-      <c r="L35" s="86"/>
-      <c r="M35" s="89">
+        <v>394</v>
+      </c>
+      <c r="K35" s="80" t="s">
+        <v>397</v>
+      </c>
+      <c r="L35" s="82"/>
+      <c r="M35" s="85">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3538,7 +3550,7 @@
       <c r="L36" s="19">
         <v>2.2599999999999998</v>
       </c>
-      <c r="M36" s="89">
+      <c r="M36" s="85">
         <f t="shared" si="3"/>
         <v>2.2599999999999998</v>
       </c>
@@ -3575,7 +3587,7 @@
       <c r="L37" s="19">
         <v>2.2599999999999998</v>
       </c>
-      <c r="M37" s="89">
+      <c r="M37" s="85">
         <f t="shared" si="3"/>
         <v>2.2599999999999998</v>
       </c>
@@ -3612,7 +3624,7 @@
       <c r="L38" s="19">
         <v>1.79</v>
       </c>
-      <c r="M38" s="89">
+      <c r="M38" s="85">
         <f t="shared" si="3"/>
         <v>1.79</v>
       </c>
@@ -3649,7 +3661,7 @@
       <c r="L39" s="19">
         <v>1.34</v>
       </c>
-      <c r="M39" s="89">
+      <c r="M39" s="85">
         <f t="shared" si="3"/>
         <v>2.68</v>
       </c>
@@ -3686,21 +3698,21 @@
       <c r="L40" s="19">
         <v>0.26</v>
       </c>
-      <c r="M40" s="89">
+      <c r="M40" s="85">
         <f t="shared" si="3"/>
         <v>0.52</v>
       </c>
     </row>
     <row r="41" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <f t="shared" si="0"/>
+        <f>A40+1</f>
         <v>35</v>
       </c>
       <c r="B41" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>346</v>
+        <v>417</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>307</v>
@@ -3724,312 +3736,312 @@
         <v>309</v>
       </c>
       <c r="K41" s="51"/>
-      <c r="L41" s="77">
+      <c r="L41" s="19">
         <v>3.5520000000000003E-2</v>
       </c>
-      <c r="M41" s="89">
+      <c r="M41" s="85">
         <f t="shared" si="3"/>
-        <v>0.10656000000000002</v>
+        <v>3.5520000000000003E-2</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
-        <f t="shared" si="0"/>
+        <f>A41+1</f>
         <v>36</v>
       </c>
       <c r="B42" s="25">
+        <v>2</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="77"/>
+      <c r="M42" s="85"/>
+    </row>
+    <row r="43" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12">
+        <f t="shared" ref="A43:A93" si="4">A42+1</f>
+        <v>37</v>
+      </c>
+      <c r="B43" s="25">
         <v>4</v>
       </c>
-      <c r="C42" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="D42" s="10" t="s">
+      <c r="C43" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="E42" s="64" t="s">
+      <c r="E43" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="F43" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="G42" s="13">
-        <v>2</v>
-      </c>
-      <c r="H42" s="14" t="s">
+      <c r="G43" s="13">
+        <v>2</v>
+      </c>
+      <c r="H43" s="14" t="s">
         <v>305</v>
       </c>
-      <c r="I42" s="10" t="s">
+      <c r="I43" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J42" s="10" t="s">
+      <c r="J43" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="K42" s="51"/>
-      <c r="L42" s="19">
+      <c r="K43" s="51"/>
+      <c r="L43" s="19">
         <v>2.8160000000000001E-2</v>
       </c>
-      <c r="M42" s="89">
+      <c r="M43" s="85">
         <f t="shared" si="3"/>
         <v>0.11264</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B43" s="25">
-        <v>2</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>348</v>
-      </c>
-      <c r="D43" s="10" t="s">
+    <row r="44" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="B44" s="25">
+        <v>2</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E43" s="59" t="s">
+      <c r="E44" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F44" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="G43" s="13">
-        <v>2</v>
-      </c>
-      <c r="H43" s="58" t="s">
+      <c r="G44" s="13">
+        <v>2</v>
+      </c>
+      <c r="H44" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="I43" s="10" t="s">
+      <c r="I44" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J43" s="58" t="s">
+      <c r="J44" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="K43" s="50" t="s">
+      <c r="K44" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="L43" s="19">
+      <c r="L44" s="19">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="M43" s="89">
+      <c r="M44" s="85">
         <f t="shared" si="3"/>
         <v>0.114</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B44" s="25">
-        <v>2</v>
-      </c>
-      <c r="C44" s="16" t="s">
+    <row r="45" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="B45" s="25">
+        <v>2</v>
+      </c>
+      <c r="C45" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D45" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E45" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F45" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G44" s="13">
-        <v>2</v>
-      </c>
-      <c r="H44" s="14" t="s">
+      <c r="G45" s="13">
+        <v>2</v>
+      </c>
+      <c r="H45" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="10" t="s">
+      <c r="I45" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J44" s="14" t="s">
+      <c r="J45" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K44" s="51" t="s">
+      <c r="K45" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="L44" s="19">
+      <c r="L45" s="19">
         <v>1.40408</v>
       </c>
-      <c r="M44" s="89">
+      <c r="M45" s="85">
         <f t="shared" si="3"/>
         <v>2.80816</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="12">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B45" s="25">
+    <row r="46" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="B46" s="25">
         <v>1</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C46" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F46" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G45" s="13">
-        <v>2</v>
-      </c>
-      <c r="H45" s="14" t="s">
+      <c r="G46" s="13">
+        <v>2</v>
+      </c>
+      <c r="H46" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="I45" s="10" t="s">
+      <c r="I46" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J45" s="14" t="s">
+      <c r="J46" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="K45" s="51" t="s">
+      <c r="K46" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="L45" s="19">
+      <c r="L46" s="19">
         <v>0.7</v>
       </c>
-      <c r="M45" s="89">
+      <c r="M46" s="85">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B46" s="25">
-        <v>2</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>349</v>
-      </c>
-      <c r="D46" s="55" t="s">
+    <row r="47" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="B47" s="25">
+        <v>2</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="D47" s="55" t="s">
         <v>314</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E47" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F46" s="67" t="s">
+      <c r="F47" s="67" t="s">
         <v>215</v>
       </c>
-      <c r="G46" s="68">
-        <v>2</v>
-      </c>
-      <c r="H46" s="69" t="s">
+      <c r="G47" s="68">
+        <v>2</v>
+      </c>
+      <c r="H47" s="69" t="s">
         <v>319</v>
       </c>
-      <c r="I46" s="70"/>
-      <c r="J46" s="71"/>
-      <c r="K46" s="50" t="s">
+      <c r="I47" s="70"/>
+      <c r="J47" s="71"/>
+      <c r="K47" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="L46" s="19">
+      <c r="L47" s="19">
         <v>6.6299999999999998E-2</v>
       </c>
-      <c r="M46" s="89">
+      <c r="M47" s="85">
         <f t="shared" si="3"/>
         <v>0.1326</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="12">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B47" s="25">
+    <row r="48" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="B48" s="25">
         <v>1</v>
       </c>
-      <c r="C47" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="D47" s="10" t="s">
+      <c r="C48" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="D48" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E48" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F48" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G47" s="13">
-        <v>2</v>
-      </c>
-      <c r="H47" s="16" t="s">
+      <c r="G48" s="13">
+        <v>2</v>
+      </c>
+      <c r="H48" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="I47" s="10" t="s">
+      <c r="I48" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J47" s="10" t="s">
+      <c r="J48" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="K47" s="51" t="s">
+      <c r="K48" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="L47" s="19">
+      <c r="L48" s="19">
         <v>0.34899999999999998</v>
       </c>
-      <c r="M47" s="89">
+      <c r="M48" s="85">
         <f t="shared" si="3"/>
         <v>0.34899999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="12">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B48" s="25">
-        <v>8</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>358</v>
-      </c>
-      <c r="D48" s="55" t="s">
-        <v>227</v>
-      </c>
-      <c r="E48" s="64" t="s">
-        <v>176</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G48" s="13">
-        <v>2</v>
-      </c>
-      <c r="H48" s="14"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="50"/>
-      <c r="L48" s="19"/>
-      <c r="M48" s="89"/>
-    </row>
     <row r="49" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="B49" s="25">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>359</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>268</v>
+        <v>357</v>
+      </c>
+      <c r="D49" s="55" t="s">
+        <v>227</v>
       </c>
       <c r="E49" s="64" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="F49" s="20" t="s">
         <v>53</v>
@@ -4042,21 +4054,21 @@
       <c r="J49" s="10"/>
       <c r="K49" s="50"/>
       <c r="L49" s="19"/>
-      <c r="M49" s="89"/>
+      <c r="M49" s="85"/>
     </row>
     <row r="50" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
       <c r="B50" s="25">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E50" s="64" t="s">
         <v>125</v>
@@ -4072,21 +4084,21 @@
       <c r="J50" s="10"/>
       <c r="K50" s="50"/>
       <c r="L50" s="19"/>
-      <c r="M50" s="89"/>
+      <c r="M50" s="85"/>
     </row>
     <row r="51" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="B51" s="25">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E51" s="64" t="s">
         <v>125</v>
@@ -4102,21 +4114,21 @@
       <c r="J51" s="10"/>
       <c r="K51" s="50"/>
       <c r="L51" s="19"/>
-      <c r="M51" s="89"/>
+      <c r="M51" s="85"/>
     </row>
     <row r="52" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
       <c r="B52" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E52" s="64" t="s">
         <v>125</v>
@@ -4132,21 +4144,21 @@
       <c r="J52" s="10"/>
       <c r="K52" s="50"/>
       <c r="L52" s="19"/>
-      <c r="M52" s="89"/>
+      <c r="M52" s="85"/>
     </row>
     <row r="53" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="B53" s="25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>408</v>
+        <v>361</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E53" s="64" t="s">
         <v>125</v>
@@ -4162,21 +4174,21 @@
       <c r="J53" s="10"/>
       <c r="K53" s="50"/>
       <c r="L53" s="19"/>
-      <c r="M53" s="89"/>
+      <c r="M53" s="85"/>
     </row>
     <row r="54" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="B54" s="79">
-        <v>10</v>
-      </c>
-      <c r="C54" s="87" t="s">
-        <v>409</v>
+      <c r="B54" s="25">
+        <v>6</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>407</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E54" s="64" t="s">
         <v>125</v>
@@ -4192,21 +4204,21 @@
       <c r="J54" s="10"/>
       <c r="K54" s="50"/>
       <c r="L54" s="19"/>
-      <c r="M54" s="89"/>
+      <c r="M54" s="85"/>
     </row>
     <row r="55" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
       <c r="B55" s="79">
-        <v>5</v>
-      </c>
-      <c r="C55" s="87" t="s">
-        <v>407</v>
+        <v>10</v>
+      </c>
+      <c r="C55" s="83" t="s">
+        <v>408</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E55" s="64" t="s">
         <v>125</v>
@@ -4222,79 +4234,79 @@
       <c r="J55" s="10"/>
       <c r="K55" s="50"/>
       <c r="L55" s="19"/>
-      <c r="M55" s="89"/>
+      <c r="M55" s="85"/>
     </row>
     <row r="56" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="B56" s="79">
-        <v>0</v>
-      </c>
-      <c r="C56" s="87" t="s">
-        <v>404</v>
-      </c>
-      <c r="D56" s="55" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="C56" s="83" t="s">
+        <v>406</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>274</v>
       </c>
       <c r="E56" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="F56" s="20"/>
+      <c r="F56" s="20" t="s">
+        <v>53</v>
+      </c>
       <c r="G56" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H56" s="14"/>
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
       <c r="K56" s="50"/>
       <c r="L56" s="19"/>
-      <c r="M56" s="89"/>
+      <c r="M56" s="85"/>
     </row>
     <row r="57" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
       <c r="B57" s="79">
-        <v>4</v>
-      </c>
-      <c r="C57" s="87" t="s">
-        <v>363</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>275</v>
+        <v>0</v>
+      </c>
+      <c r="C57" s="83" t="s">
+        <v>403</v>
+      </c>
+      <c r="D57" s="55" t="s">
+        <v>0</v>
       </c>
       <c r="E57" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="F57" s="20" t="s">
-        <v>53</v>
-      </c>
+      <c r="F57" s="20"/>
       <c r="G57" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H57" s="14"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="50"/>
       <c r="L57" s="19"/>
-      <c r="M57" s="89"/>
+      <c r="M57" s="85"/>
     </row>
     <row r="58" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
-      <c r="B58" s="25">
-        <v>2</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>364</v>
+      <c r="B58" s="79">
+        <v>4</v>
+      </c>
+      <c r="C58" s="83" t="s">
+        <v>362</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E58" s="64" t="s">
         <v>125</v>
@@ -4310,21 +4322,21 @@
       <c r="J58" s="10"/>
       <c r="K58" s="50"/>
       <c r="L58" s="19"/>
-      <c r="M58" s="89"/>
+      <c r="M58" s="85"/>
     </row>
     <row r="59" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="B59" s="78">
-        <v>11</v>
-      </c>
-      <c r="C59" s="63" t="s">
-        <v>365</v>
+      <c r="B59" s="25">
+        <v>2</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>363</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E59" s="64" t="s">
         <v>125</v>
@@ -4340,21 +4352,21 @@
       <c r="J59" s="10"/>
       <c r="K59" s="50"/>
       <c r="L59" s="19"/>
-      <c r="M59" s="89"/>
+      <c r="M59" s="85"/>
     </row>
     <row r="60" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="B60" s="78">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C60" s="63" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E60" s="64" t="s">
         <v>125</v>
@@ -4370,21 +4382,21 @@
       <c r="J60" s="10"/>
       <c r="K60" s="50"/>
       <c r="L60" s="19"/>
-      <c r="M60" s="89"/>
+      <c r="M60" s="85"/>
     </row>
     <row r="61" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="B61" s="25">
-        <v>2</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>367</v>
+      <c r="B61" s="78">
+        <v>2</v>
+      </c>
+      <c r="C61" s="63" t="s">
+        <v>365</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E61" s="64" t="s">
         <v>125</v>
@@ -4400,21 +4412,21 @@
       <c r="J61" s="10"/>
       <c r="K61" s="50"/>
       <c r="L61" s="19"/>
-      <c r="M61" s="89"/>
+      <c r="M61" s="85"/>
     </row>
     <row r="62" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="B62" s="25">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E62" s="64" t="s">
         <v>125</v>
@@ -4430,21 +4442,21 @@
       <c r="J62" s="10"/>
       <c r="K62" s="50"/>
       <c r="L62" s="19"/>
-      <c r="M62" s="89"/>
+      <c r="M62" s="85"/>
     </row>
     <row r="63" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
       <c r="B63" s="25">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E63" s="64" t="s">
         <v>125</v>
@@ -4460,21 +4472,21 @@
       <c r="J63" s="10"/>
       <c r="K63" s="50"/>
       <c r="L63" s="19"/>
-      <c r="M63" s="89"/>
+      <c r="M63" s="85"/>
     </row>
     <row r="64" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="B64" s="25">
         <v>1</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>370</v>
-      </c>
-      <c r="D64" s="66" t="s">
-        <v>320</v>
+        <v>368</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="E64" s="64" t="s">
         <v>125</v>
@@ -4490,21 +4502,21 @@
       <c r="J64" s="10"/>
       <c r="K64" s="50"/>
       <c r="L64" s="19"/>
-      <c r="M64" s="89"/>
+      <c r="M64" s="85"/>
     </row>
     <row r="65" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
       <c r="B65" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D65" s="66" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="E65" s="64" t="s">
         <v>125</v>
@@ -4520,58 +4532,51 @@
       <c r="J65" s="10"/>
       <c r="K65" s="50"/>
       <c r="L65" s="19"/>
-      <c r="M65" s="89"/>
+      <c r="M65" s="85"/>
     </row>
     <row r="66" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="B66" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>372</v>
-      </c>
-      <c r="D66" s="20" t="s">
-        <v>226</v>
+        <v>370</v>
+      </c>
+      <c r="D66" s="66" t="s">
+        <v>282</v>
       </c>
       <c r="E66" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="F66" s="20"/>
+      <c r="F66" s="20" t="s">
+        <v>53</v>
+      </c>
       <c r="G66" s="13">
         <v>2</v>
       </c>
-      <c r="H66" s="14" t="s">
-        <v>260</v>
-      </c>
+      <c r="H66" s="14"/>
       <c r="I66" s="10"/>
-      <c r="J66" s="10" t="s">
-        <v>261</v>
-      </c>
+      <c r="J66" s="10"/>
       <c r="K66" s="50"/>
-      <c r="L66" s="19">
-        <v>0.2077</v>
-      </c>
-      <c r="M66" s="89">
-        <f t="shared" ref="M66:M92" si="4">B66*L66</f>
-        <v>0.2077</v>
-      </c>
+      <c r="L66" s="19"/>
+      <c r="M66" s="85"/>
     </row>
     <row r="67" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="B67" s="25">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E67" s="64" t="s">
         <v>125</v>
@@ -4581,34 +4586,34 @@
         <v>2</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I67" s="10"/>
       <c r="J67" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K67" s="50"/>
       <c r="L67" s="19">
-        <v>0.11693000000000001</v>
-      </c>
-      <c r="M67" s="89">
-        <f t="shared" si="4"/>
-        <v>0.81851000000000007</v>
+        <v>0.2077</v>
+      </c>
+      <c r="M67" s="85">
+        <f t="shared" ref="M67:M93" si="5">B67*L67</f>
+        <v>0.2077</v>
       </c>
     </row>
     <row r="68" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="B68" s="25">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C68" s="16" t="s">
         <v>376</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>355</v>
+        <v>224</v>
       </c>
       <c r="E68" s="64" t="s">
         <v>125</v>
@@ -4618,34 +4623,34 @@
         <v>2</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>356</v>
+        <v>263</v>
       </c>
       <c r="I68" s="10"/>
       <c r="J68" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="K68" s="51"/>
+        <v>262</v>
+      </c>
+      <c r="K68" s="50"/>
       <c r="L68" s="19">
-        <v>0.62</v>
-      </c>
-      <c r="M68" s="89">
-        <f t="shared" si="4"/>
-        <v>0.62</v>
+        <v>0.11693000000000001</v>
+      </c>
+      <c r="M68" s="85">
+        <f t="shared" si="5"/>
+        <v>0.81851000000000007</v>
       </c>
     </row>
     <row r="69" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="B69" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>225</v>
+        <v>354</v>
       </c>
       <c r="E69" s="64" t="s">
         <v>125</v>
@@ -4655,34 +4660,34 @@
         <v>2</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>264</v>
+        <v>355</v>
       </c>
       <c r="I69" s="10"/>
       <c r="J69" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="K69" s="50"/>
+        <v>356</v>
+      </c>
+      <c r="K69" s="51"/>
       <c r="L69" s="19">
-        <v>0.2041</v>
-      </c>
-      <c r="M69" s="89">
-        <f t="shared" si="4"/>
-        <v>0.40820000000000001</v>
+        <v>0.62</v>
+      </c>
+      <c r="M69" s="85">
+        <f t="shared" si="5"/>
+        <v>0.62</v>
       </c>
     </row>
     <row r="70" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="B70" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E70" s="64" t="s">
         <v>125</v>
@@ -4692,652 +4697,646 @@
         <v>2</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I70" s="10"/>
       <c r="J70" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K70" s="50"/>
-      <c r="L70" s="77">
+      <c r="L70" s="19">
         <v>0.2041</v>
       </c>
-      <c r="M70" s="89">
-        <f t="shared" si="4"/>
-        <v>0.2041</v>
+      <c r="M70" s="85">
+        <f t="shared" si="5"/>
+        <v>0.40820000000000001</v>
       </c>
     </row>
     <row r="71" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="B71" s="25">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D71" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E71" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F71" s="20" t="s">
-        <v>68</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="E71" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="F71" s="20"/>
       <c r="G71" s="13">
         <v>2</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I71" s="10" t="s">
-        <v>52</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="I71" s="10"/>
       <c r="J71" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="K71" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="L71" s="19">
-        <v>2.4E-2</v>
-      </c>
-      <c r="M71" s="89">
-        <f t="shared" si="4"/>
-        <v>0.192</v>
+        <v>267</v>
+      </c>
+      <c r="K71" s="50"/>
+      <c r="L71" s="77">
+        <v>0.2041</v>
+      </c>
+      <c r="M71" s="85">
+        <f t="shared" si="5"/>
+        <v>0.2041</v>
       </c>
     </row>
     <row r="72" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
       <c r="B72" s="25">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>410</v>
+        <v>374</v>
       </c>
       <c r="D72" s="20" t="s">
-        <v>411</v>
+        <v>97</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F72" s="20"/>
+        <v>51</v>
+      </c>
+      <c r="F72" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="G72" s="13">
         <v>2</v>
       </c>
-      <c r="H72" s="10" t="s">
-        <v>413</v>
+      <c r="H72" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="I72" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="K72" s="51"/>
+        <v>67</v>
+      </c>
+      <c r="K72" s="51" t="s">
+        <v>84</v>
+      </c>
       <c r="L72" s="19">
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="M72" s="89">
-        <f t="shared" si="4"/>
-        <v>0.46800000000000003</v>
+        <v>2.4E-2</v>
+      </c>
+      <c r="M72" s="85">
+        <f t="shared" si="5"/>
+        <v>0.192</v>
       </c>
     </row>
     <row r="73" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12">
-        <f>A72+1</f>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="B73" s="25">
         <v>2</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D73" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>75</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>410</v>
+      </c>
+      <c r="E73" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F73" s="20"/>
       <c r="G73" s="13">
         <v>2</v>
       </c>
       <c r="H73" s="10" t="s">
-        <v>140</v>
+        <v>412</v>
       </c>
       <c r="I73" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="K73" s="60" t="s">
-        <v>177</v>
-      </c>
-      <c r="L73" s="11">
-        <v>5.9400000000000001E-2</v>
-      </c>
-      <c r="M73" s="89">
-        <f t="shared" si="4"/>
-        <v>0.1188</v>
+        <v>411</v>
+      </c>
+      <c r="K73" s="51"/>
+      <c r="L73" s="19">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="M73" s="85">
+        <f t="shared" si="5"/>
+        <v>0.46800000000000003</v>
       </c>
     </row>
     <row r="74" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
-        <f>A73+1</f>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="B74" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>60</v>
+        <v>158</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G74" s="13">
         <v>2</v>
       </c>
-      <c r="H74" s="16" t="s">
-        <v>31</v>
+      <c r="H74" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="I74" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K74" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="L74" s="19">
-        <v>2.48</v>
-      </c>
-      <c r="M74" s="89">
-        <f t="shared" si="4"/>
-        <v>2.48</v>
+        <v>141</v>
+      </c>
+      <c r="K74" s="60" t="s">
+        <v>177</v>
+      </c>
+      <c r="L74" s="11">
+        <v>5.9400000000000001E-2</v>
+      </c>
+      <c r="M74" s="85">
+        <f t="shared" si="5"/>
+        <v>0.1188</v>
       </c>
     </row>
     <row r="75" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
-        <f>A74+1</f>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="B75" s="25">
         <v>1</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D75" s="55" t="s">
-        <v>220</v>
+        <v>60</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="F75" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="G75" s="37"/>
-      <c r="H75" s="10" t="s">
-        <v>200</v>
+        <v>71</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G75" s="13">
+        <v>2</v>
+      </c>
+      <c r="H75" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="I75" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J75" s="62" t="s">
-        <v>201</v>
-      </c>
-      <c r="K75" s="62"/>
+      <c r="J75" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K75" s="61" t="s">
+        <v>92</v>
+      </c>
       <c r="L75" s="19">
-        <v>198</v>
-      </c>
-      <c r="M75" s="89">
-        <f t="shared" si="4"/>
-        <v>198</v>
+        <v>2.48</v>
+      </c>
+      <c r="M75" s="85">
+        <f t="shared" si="5"/>
+        <v>2.48</v>
       </c>
     </row>
     <row r="76" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
-        <f t="shared" ref="A76:A86" si="5">A75+1</f>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="B76" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="D76" s="55" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="G76" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="H76" s="14" t="s">
-        <v>189</v>
+        <v>79</v>
+      </c>
+      <c r="G76" s="37"/>
+      <c r="H76" s="10" t="s">
+        <v>200</v>
       </c>
       <c r="I76" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J76" s="10" t="s">
-        <v>188</v>
+      <c r="J76" s="62" t="s">
+        <v>201</v>
       </c>
       <c r="K76" s="62"/>
       <c r="L76" s="19">
-        <v>8.6430000000000007</v>
-      </c>
-      <c r="M76" s="89">
-        <f t="shared" si="4"/>
-        <v>17.286000000000001</v>
+        <v>198</v>
+      </c>
+      <c r="M76" s="85">
+        <f t="shared" si="5"/>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="B77" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="D77" s="55" t="s">
-        <v>394</v>
+        <v>221</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="G77" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H77" s="51" t="s">
-        <v>392</v>
-      </c>
-      <c r="I77" s="10"/>
-      <c r="J77" s="51" t="s">
-        <v>393</v>
+      <c r="H77" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="I77" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J77" s="10" t="s">
+        <v>188</v>
       </c>
       <c r="K77" s="62"/>
-      <c r="L77" s="77">
-        <v>1.4827999999999999</v>
-      </c>
-      <c r="M77" s="89">
-        <f t="shared" si="4"/>
-        <v>1.4827999999999999</v>
+      <c r="L77" s="19">
+        <v>8.6430000000000007</v>
+      </c>
+      <c r="M77" s="85">
+        <f t="shared" si="5"/>
+        <v>17.286000000000001</v>
       </c>
     </row>
     <row r="78" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="B78" s="25">
         <v>1</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E78" s="21" t="s">
-        <v>62</v>
+        <v>122</v>
+      </c>
+      <c r="D78" s="55" t="s">
+        <v>393</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G78" s="37"/>
-      <c r="H78" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I78" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J78" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="K78" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="L78" s="19">
-        <v>5.5456000000000003</v>
-      </c>
-      <c r="M78" s="89">
-        <f t="shared" si="4"/>
-        <v>5.5456000000000003</v>
+        <v>202</v>
+      </c>
+      <c r="G78" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H78" s="51" t="s">
+        <v>391</v>
+      </c>
+      <c r="I78" s="10"/>
+      <c r="J78" s="51" t="s">
+        <v>392</v>
+      </c>
+      <c r="K78" s="62"/>
+      <c r="L78" s="77">
+        <v>1.4827999999999999</v>
+      </c>
+      <c r="M78" s="85">
+        <f t="shared" si="5"/>
+        <v>1.4827999999999999</v>
       </c>
     </row>
     <row r="79" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="B79" s="25">
         <v>1</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D79" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="E79" s="14" t="s">
-        <v>108</v>
+        <v>163</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E79" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="F79" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="G79" s="13"/>
-      <c r="H79" s="55" t="s">
-        <v>118</v>
+      <c r="G79" s="37"/>
+      <c r="H79" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="I79" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J79" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="K79" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="L79" s="11">
-        <v>0.67900000000000005</v>
-      </c>
-      <c r="M79" s="89">
-        <f t="shared" si="4"/>
-        <v>0.67900000000000005</v>
+      <c r="J79" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K79" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="L79" s="19">
+        <v>5.5456000000000003</v>
+      </c>
+      <c r="M79" s="85">
+        <f t="shared" si="5"/>
+        <v>5.5456000000000003</v>
       </c>
     </row>
     <row r="80" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="B80" s="25">
         <v>1</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D80" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="E80" s="21" t="s">
-        <v>65</v>
+        <v>164</v>
+      </c>
+      <c r="D80" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="G80" s="13">
-        <v>2</v>
-      </c>
-      <c r="H80" s="20" t="s">
-        <v>106</v>
+        <v>76</v>
+      </c>
+      <c r="G80" s="13"/>
+      <c r="H80" s="55" t="s">
+        <v>118</v>
       </c>
       <c r="I80" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J80" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="K80" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="L80" s="19">
-        <v>1.3068</v>
-      </c>
-      <c r="M80" s="89">
-        <f t="shared" si="4"/>
-        <v>1.3068</v>
+        <v>119</v>
+      </c>
+      <c r="K80" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="L80" s="11">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="M80" s="85">
+        <f t="shared" si="5"/>
+        <v>0.67900000000000005</v>
       </c>
     </row>
     <row r="81" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="B81" s="25">
         <v>1</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="D81" s="55" t="s">
-        <v>205</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>108</v>
+        <v>64</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E81" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="G81" s="13">
         <v>2</v>
       </c>
-      <c r="H81" s="14" t="s">
-        <v>204</v>
+      <c r="H81" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="I81" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J81" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="K81" s="62"/>
+      <c r="J81" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="K81" s="61" t="s">
+        <v>91</v>
+      </c>
       <c r="L81" s="19">
-        <v>0.86060000000000003</v>
-      </c>
-      <c r="M81" s="89">
-        <f t="shared" si="4"/>
-        <v>0.86060000000000003</v>
+        <v>1.3068</v>
+      </c>
+      <c r="M81" s="85">
+        <f t="shared" si="5"/>
+        <v>1.3068</v>
       </c>
     </row>
     <row r="82" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
       <c r="B82" s="25">
         <v>1</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D82" s="55" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>108</v>
       </c>
       <c r="F82" s="20" t="s">
-        <v>215</v>
+        <v>76</v>
       </c>
       <c r="G82" s="13">
         <v>2</v>
       </c>
       <c r="H82" s="14" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="I82" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="K82" s="62"/>
-      <c r="L82" s="77">
-        <v>0.21909999999999999</v>
-      </c>
-      <c r="M82" s="89">
-        <f t="shared" si="4"/>
-        <v>0.21909999999999999</v>
+      <c r="L82" s="19">
+        <v>0.86060000000000003</v>
+      </c>
+      <c r="M82" s="85">
+        <f t="shared" si="5"/>
+        <v>0.86060000000000003</v>
       </c>
     </row>
     <row r="83" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12">
+        <f t="shared" si="4"/>
+        <v>77</v>
+      </c>
+      <c r="B83" s="25">
+        <v>1</v>
+      </c>
+      <c r="C83" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D83" s="55" t="s">
+        <v>216</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F83" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="G83" s="13">
+        <v>2</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="I83" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J83" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="K83" s="62"/>
+      <c r="L83" s="77">
+        <v>0.21909999999999999</v>
+      </c>
+      <c r="M83" s="85">
         <f t="shared" si="5"/>
-        <v>77</v>
-      </c>
-      <c r="B83" s="25">
-        <v>2</v>
-      </c>
-      <c r="C83" s="16" t="s">
-        <v>351</v>
-      </c>
-      <c r="D83" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="E83" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="F83" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="G83" s="13"/>
-      <c r="H83" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="I83" s="10"/>
-      <c r="J83" s="10"/>
-      <c r="K83" s="62"/>
-      <c r="L83" s="19">
-        <v>3.5903999999999998</v>
-      </c>
-      <c r="M83" s="89">
-        <f t="shared" si="4"/>
-        <v>7.1807999999999996</v>
+        <v>0.21909999999999999</v>
       </c>
     </row>
     <row r="84" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12">
+        <f t="shared" si="4"/>
+        <v>78</v>
+      </c>
+      <c r="B84" s="25">
+        <v>2</v>
+      </c>
+      <c r="C84" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F84" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="G84" s="13"/>
+      <c r="H84" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="62"/>
+      <c r="L84" s="19">
+        <v>3.5903999999999998</v>
+      </c>
+      <c r="M84" s="85">
         <f t="shared" si="5"/>
-        <v>78</v>
-      </c>
-      <c r="B84" s="25">
-        <v>2</v>
-      </c>
-      <c r="C84" s="16" t="s">
-        <v>352</v>
-      </c>
-      <c r="D84" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E84" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F84" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G84" s="13">
-        <v>1</v>
-      </c>
-      <c r="H84" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I84" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="J84" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K84" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="L84" s="19">
-        <v>3.39</v>
-      </c>
-      <c r="M84" s="89">
-        <f t="shared" si="4"/>
-        <v>6.78</v>
+        <v>7.1807999999999996</v>
       </c>
     </row>
     <row r="85" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>79</v>
       </c>
       <c r="B85" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>353</v>
-      </c>
-      <c r="D85" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E85" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="F85" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F85" s="20" t="s">
         <v>77</v>
       </c>
       <c r="G85" s="13">
         <v>1</v>
       </c>
-      <c r="H85" s="58" t="s">
-        <v>127</v>
+      <c r="H85" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="I85" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J85" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="K85" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="L85" s="11">
-        <v>4.28</v>
-      </c>
-      <c r="M85" s="89">
-        <f t="shared" si="4"/>
-        <v>4.28</v>
+      <c r="J85" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K85" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="L85" s="19">
+        <v>3.39</v>
+      </c>
+      <c r="M85" s="85">
+        <f t="shared" si="5"/>
+        <v>6.78</v>
       </c>
     </row>
     <row r="86" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="B86" s="25">
         <v>1</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E86" s="10" t="s">
-        <v>170</v>
+        <v>126</v>
+      </c>
+      <c r="E86" s="58" t="s">
+        <v>124</v>
       </c>
       <c r="F86" s="10" t="s">
         <v>77</v>
@@ -5345,40 +5344,42 @@
       <c r="G86" s="13">
         <v>1</v>
       </c>
-      <c r="H86" s="14" t="s">
-        <v>190</v>
+      <c r="H86" s="58" t="s">
+        <v>127</v>
       </c>
       <c r="I86" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J86" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="K86" s="62"/>
-      <c r="L86" s="19">
-        <v>5.62263</v>
-      </c>
-      <c r="M86" s="89">
-        <f t="shared" si="4"/>
-        <v>5.62263</v>
+        <v>77</v>
+      </c>
+      <c r="J86" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="K86" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="L86" s="11">
+        <v>4.28</v>
+      </c>
+      <c r="M86" s="85">
+        <f t="shared" si="5"/>
+        <v>4.28</v>
       </c>
     </row>
     <row r="87" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12">
-        <f t="shared" ref="A87:A92" si="6">A86+1</f>
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
       <c r="B87" s="25">
         <v>1</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>222</v>
+        <v>353</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F87" s="10" t="s">
         <v>77</v>
@@ -5387,39 +5388,39 @@
         <v>1</v>
       </c>
       <c r="H87" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I87" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J87" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K87" s="62"/>
       <c r="L87" s="19">
-        <v>8.8635999999999999</v>
-      </c>
-      <c r="M87" s="89">
-        <f t="shared" si="4"/>
-        <v>8.8635999999999999</v>
+        <v>5.62263</v>
+      </c>
+      <c r="M87" s="85">
+        <f t="shared" si="5"/>
+        <v>5.62263</v>
       </c>
     </row>
     <row r="88" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="B88" s="25">
         <v>1</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="D88" s="55" t="s">
-        <v>208</v>
+        <v>222</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F88" s="10" t="s">
         <v>77</v>
@@ -5428,327 +5429,373 @@
         <v>1</v>
       </c>
       <c r="H88" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="I88" s="10"/>
+        <v>191</v>
+      </c>
+      <c r="I88" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="J88" s="10" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="K88" s="62"/>
-      <c r="L88" s="77">
-        <v>5.0944000000000003</v>
-      </c>
-      <c r="M88" s="89">
-        <f t="shared" si="4"/>
-        <v>5.0944000000000003</v>
+      <c r="L88" s="19">
+        <v>8.8635999999999999</v>
+      </c>
+      <c r="M88" s="85">
+        <f t="shared" si="5"/>
+        <v>8.8635999999999999</v>
       </c>
     </row>
     <row r="89" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>83</v>
       </c>
       <c r="B89" s="25">
         <v>1</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>199</v>
+        <v>168</v>
+      </c>
+      <c r="D89" s="55" t="s">
+        <v>208</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F89" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G89" s="13"/>
+        <v>174</v>
+      </c>
+      <c r="F89" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G89" s="13">
+        <v>1</v>
+      </c>
       <c r="H89" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="I89" s="10" t="s">
-        <v>52</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="I89" s="10"/>
       <c r="J89" s="10" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="K89" s="62"/>
-      <c r="L89" s="19">
-        <v>1.4631000000000001</v>
-      </c>
-      <c r="M89" s="89">
-        <f t="shared" si="4"/>
-        <v>1.4631000000000001</v>
+      <c r="L89" s="77">
+        <v>5.0944000000000003</v>
+      </c>
+      <c r="M89" s="85">
+        <f t="shared" si="5"/>
+        <v>5.0944000000000003</v>
       </c>
     </row>
     <row r="90" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="B90" s="25">
         <v>1</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="D90" s="66" t="s">
-        <v>416</v>
-      </c>
-      <c r="E90" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="F90" s="66" t="s">
-        <v>318</v>
-      </c>
-      <c r="G90" s="13">
-        <v>2</v>
-      </c>
-      <c r="H90" s="10" t="s">
-        <v>316</v>
+        <v>169</v>
+      </c>
+      <c r="D90" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F90" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G90" s="13"/>
+      <c r="H90" s="14" t="s">
+        <v>192</v>
       </c>
       <c r="I90" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J90" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="K90" s="60" t="s">
-        <v>180</v>
-      </c>
-      <c r="L90" s="11">
-        <v>1.1088</v>
-      </c>
-      <c r="M90" s="89">
-        <f t="shared" si="4"/>
-        <v>1.1088</v>
+        <v>187</v>
+      </c>
+      <c r="K90" s="62"/>
+      <c r="L90" s="19">
+        <v>1.4631000000000001</v>
+      </c>
+      <c r="M90" s="85">
+        <f t="shared" si="5"/>
+        <v>1.4631000000000001</v>
       </c>
     </row>
     <row r="91" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>85</v>
       </c>
       <c r="B91" s="25">
         <v>1</v>
       </c>
       <c r="C91" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D91" s="66" t="s">
         <v>415</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="E91" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F91" s="20" t="s">
+      <c r="F91" s="66" t="s">
+        <v>318</v>
+      </c>
+      <c r="G91" s="13">
+        <v>2</v>
+      </c>
+      <c r="H91" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="I91" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J91" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="K91" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="L91" s="11">
+        <v>1.1088</v>
+      </c>
+      <c r="M91" s="85">
+        <f t="shared" si="5"/>
+        <v>1.1088</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="12">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="B92" s="25">
+        <v>1</v>
+      </c>
+      <c r="C92" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D92" s="66" t="s">
+        <v>414</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F92" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="G91" s="13">
-        <v>2</v>
-      </c>
-      <c r="H91" s="14" t="s">
+      <c r="G92" s="13">
+        <v>2</v>
+      </c>
+      <c r="H92" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="I91" s="10"/>
-      <c r="J91" s="55" t="s">
+      <c r="I92" s="10"/>
+      <c r="J92" s="55" t="s">
         <v>218</v>
       </c>
-      <c r="K91" s="50"/>
-      <c r="L91" s="77">
+      <c r="K92" s="50"/>
+      <c r="L92" s="77">
         <v>1.1577999999999999</v>
       </c>
-      <c r="M91" s="89">
+      <c r="M92" s="85">
+        <f t="shared" si="5"/>
+        <v>1.1577999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" s="24" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="12">
         <f t="shared" si="4"/>
-        <v>1.1577999999999999</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" s="24" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="12">
-        <f t="shared" si="6"/>
-        <v>86</v>
-      </c>
-      <c r="B92" s="29">
+        <v>87</v>
+      </c>
+      <c r="B93" s="29">
         <v>1</v>
       </c>
-      <c r="C92" s="30"/>
-      <c r="D92" s="73" t="s">
-        <v>414</v>
-      </c>
-      <c r="E92" s="32"/>
-      <c r="F92" s="31"/>
-      <c r="G92" s="33"/>
-      <c r="H92" s="30"/>
-      <c r="I92" s="31"/>
-      <c r="J92" s="31"/>
-      <c r="K92" s="52"/>
-      <c r="L92" s="34">
+      <c r="C93" s="30"/>
+      <c r="D93" s="73" t="s">
+        <v>413</v>
+      </c>
+      <c r="E93" s="32"/>
+      <c r="F93" s="31"/>
+      <c r="G93" s="33"/>
+      <c r="H93" s="30"/>
+      <c r="I93" s="31"/>
+      <c r="J93" s="31"/>
+      <c r="K93" s="52"/>
+      <c r="L93" s="34">
         <v>25</v>
       </c>
-      <c r="M92" s="90">
-        <f t="shared" si="4"/>
+      <c r="M93" s="86">
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B93">
-        <f>SUM(B7:B92)</f>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <f>SUM(B7:B93)</f>
         <v>402</v>
       </c>
-      <c r="K93" s="28" t="s">
+      <c r="K94" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="M93" s="36">
-        <f>SUM(M7:M92)</f>
-        <v>385.02645758620685</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K94" s="28"/>
-      <c r="M94" s="65"/>
-    </row>
-    <row r="96" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="26" t="s">
+      <c r="M94" s="36">
+        <f>SUM(M7:M93)</f>
+        <v>384.95541758620681</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K95" s="28"/>
+      <c r="M95" s="65"/>
+    </row>
+    <row r="97" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="26" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="26"/>
-      <c r="B97" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="C97" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="D97" s="80"/>
-      <c r="E97" s="80"/>
-      <c r="F97" s="80"/>
-      <c r="G97" s="80"/>
-      <c r="H97" s="80"/>
     </row>
     <row r="98" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="26"/>
       <c r="B98" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C98" s="76" t="s">
-        <v>322</v>
-      </c>
-      <c r="D98" s="72"/>
-      <c r="E98" s="72"/>
-      <c r="F98" s="72"/>
-      <c r="G98" s="72"/>
-      <c r="H98" s="72"/>
-      <c r="I98" s="72"/>
-      <c r="J98" s="27"/>
+      <c r="C98" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="D98" s="87"/>
+      <c r="E98" s="87"/>
+      <c r="F98" s="87"/>
+      <c r="G98" s="87"/>
+      <c r="H98" s="87"/>
     </row>
     <row r="99" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="26"/>
       <c r="B99" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C99" s="81" t="s">
+      <c r="C99" s="76" t="s">
+        <v>322</v>
+      </c>
+      <c r="D99" s="72"/>
+      <c r="E99" s="72"/>
+      <c r="F99" s="72"/>
+      <c r="G99" s="72"/>
+      <c r="H99" s="72"/>
+      <c r="I99" s="72"/>
+      <c r="J99" s="27"/>
+    </row>
+    <row r="100" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="26"/>
+      <c r="B100" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C100" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="D99" s="81"/>
-      <c r="E99" s="81"/>
-      <c r="F99" s="81"/>
-      <c r="G99" s="81"/>
-      <c r="H99" s="81"/>
-    </row>
-    <row r="100" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="38" t="s">
+      <c r="D100" s="88"/>
+      <c r="E100" s="88"/>
+      <c r="F100" s="88"/>
+      <c r="G100" s="88"/>
+      <c r="H100" s="88"/>
+    </row>
+    <row r="101" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C100" s="82" t="s">
+      <c r="C101" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="D100" s="81"/>
-      <c r="E100" s="81"/>
-      <c r="F100" s="81"/>
-      <c r="G100" s="81"/>
-      <c r="H100" s="81"/>
-    </row>
-    <row r="101" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="9">
+      <c r="D101" s="88"/>
+      <c r="E101" s="88"/>
+      <c r="F101" s="88"/>
+      <c r="G101" s="88"/>
+      <c r="H101" s="88"/>
+    </row>
+    <row r="102" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="9">
         <v>1</v>
       </c>
-      <c r="C101" s="81" t="s">
+      <c r="C102" s="88" t="s">
         <v>102</v>
       </c>
-      <c r="D101" s="81"/>
-      <c r="E101" s="81"/>
-      <c r="F101" s="81"/>
-      <c r="G101" s="81"/>
-      <c r="H101" s="81"/>
-    </row>
-    <row r="102" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="9"/>
-      <c r="C102" s="83" t="s">
-        <v>103</v>
-      </c>
-      <c r="D102" s="83"/>
-      <c r="E102" s="83"/>
-      <c r="F102" s="83"/>
-      <c r="G102" s="83"/>
-      <c r="H102" s="83"/>
+      <c r="D102" s="88"/>
+      <c r="E102" s="88"/>
+      <c r="F102" s="88"/>
+      <c r="G102" s="88"/>
+      <c r="H102" s="88"/>
     </row>
     <row r="103" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="9"/>
-      <c r="C103" s="83" t="s">
+      <c r="C103" s="90" t="s">
+        <v>103</v>
+      </c>
+      <c r="D103" s="90"/>
+      <c r="E103" s="90"/>
+      <c r="F103" s="90"/>
+      <c r="G103" s="90"/>
+      <c r="H103" s="90"/>
+    </row>
+    <row r="104" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="9"/>
+      <c r="C104" s="90" t="s">
         <v>96</v>
       </c>
-      <c r="D103" s="83"/>
-      <c r="E103" s="83"/>
-      <c r="F103" s="83"/>
-      <c r="G103" s="83"/>
-      <c r="H103" s="83"/>
-    </row>
-    <row r="104" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="9">
-        <v>2</v>
-      </c>
-      <c r="C104" s="81" t="s">
+      <c r="D104" s="90"/>
+      <c r="E104" s="90"/>
+      <c r="F104" s="90"/>
+      <c r="G104" s="90"/>
+      <c r="H104" s="90"/>
+    </row>
+    <row r="105" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="9">
+        <v>2</v>
+      </c>
+      <c r="C105" s="88" t="s">
         <v>104</v>
       </c>
-      <c r="D104" s="81"/>
-      <c r="E104" s="81"/>
-      <c r="F104" s="81"/>
-      <c r="G104" s="81"/>
-      <c r="H104" s="81"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B105" s="9">
-        <v>3</v>
-      </c>
-      <c r="C105" s="56" t="s">
-        <v>405</v>
-      </c>
+      <c r="D105" s="88"/>
+      <c r="E105" s="88"/>
+      <c r="F105" s="88"/>
+      <c r="G105" s="88"/>
+      <c r="H105" s="88"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B106" s="9">
+        <v>3</v>
+      </c>
+      <c r="C106" s="56" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B107" s="9">
         <v>4</v>
       </c>
-      <c r="C106" s="75" t="s">
+      <c r="C107" s="75" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B107" s="6"/>
-    </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B108" s="6"/>
+      <c r="B108" s="9">
+        <v>5</v>
+      </c>
+      <c r="C108" s="75" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B109" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C97:H97"/>
-    <mergeCell ref="C99:H99"/>
+    <mergeCell ref="C98:H98"/>
     <mergeCell ref="C100:H100"/>
-    <mergeCell ref="C104:H104"/>
     <mergeCell ref="C101:H101"/>
+    <mergeCell ref="C105:H105"/>
     <mergeCell ref="C102:H102"/>
     <mergeCell ref="C103:H103"/>
+    <mergeCell ref="C104:H104"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Rev 3.2: Removed L9-10, added C77-78, test points on bottom side
</commit_message>
<xml_diff>
--- a/FPGA1394V3-BOM.xlsx
+++ b/FPGA1394V3-BOM.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="420">
   <si>
     <t>Do Not Install</t>
   </si>
@@ -707,9 +707,6 @@
     <t>IC, Quad Step-Down DC-DC Converter, LTC3644</t>
   </si>
   <si>
-    <t>IS, Dual Steo-Down DC-DC Converter, LTC3636</t>
-  </si>
-  <si>
     <t>IC, DDR Termination Power Supply, LP2998</t>
   </si>
   <si>
@@ -1368,9 +1365,6 @@
     <t>1840-1011-ND</t>
   </si>
   <si>
-    <t>IEEE-1394/Ethernet FPGA Board, Rev 3.1</t>
-  </si>
-  <si>
     <t>H10245-ND</t>
   </si>
   <si>
@@ -1484,19 +1478,22 @@
     <t>IC, Crystal Oscillator, 25.00MHz</t>
   </si>
   <si>
-    <t>L9-10</t>
-  </si>
-  <si>
     <t>L8</t>
   </si>
   <si>
-    <t>RES, 0</t>
-  </si>
-  <si>
-    <t>2, 5</t>
-  </si>
-  <si>
     <t>L9-10 have been replaced by 0 Ohm resistors</t>
+  </si>
+  <si>
+    <t>IEEE-1394/Ethernet FPGA Board, Rev 3.2</t>
+  </si>
+  <si>
+    <t>C77-78</t>
+  </si>
+  <si>
+    <t>IC, Dual Step-Down DC-DC Converter, LTC3636</t>
+  </si>
+  <si>
+    <t>CAP, 4700pF, 10%, 16V, X7R, 0402</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -1934,6 +1931,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2267,7 +2265,7 @@
     <row r="1" spans="1:13" ht="29.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>385</v>
+        <v>416</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2282,7 +2280,7 @@
     <row r="2" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2297,7 +2295,7 @@
     <row r="3" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="22">
-        <v>45050</v>
+        <v>45569</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2315,7 +2313,7 @@
       </c>
       <c r="B4" s="40"/>
       <c r="C4" s="54">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="17"/>
@@ -2391,7 +2389,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>175</v>
@@ -2414,14 +2412,14 @@
     </row>
     <row r="8" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
-        <f t="shared" ref="A8:A73" si="0">A7+1</f>
+        <f t="shared" ref="A8:A21" si="0">A7+1</f>
         <v>2</v>
       </c>
       <c r="B8" s="25">
         <v>2</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>6</v>
@@ -2464,10 +2462,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>125</v>
@@ -2494,10 +2492,10 @@
         <v>21</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>125</v>
@@ -2526,10 +2524,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D11" s="55" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>125</v>
@@ -2541,11 +2539,11 @@
         <v>2</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K11" s="50"/>
       <c r="L11" s="19"/>
@@ -2560,26 +2558,26 @@
         <v>5</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D12" s="55" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>54</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G12" s="13">
         <v>2</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K12" s="50"/>
       <c r="L12" s="77">
@@ -2599,26 +2597,26 @@
         <v>13</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G13" s="13">
         <v>2</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K13" s="50"/>
       <c r="L13" s="19">
@@ -2638,26 +2636,26 @@
         <v>2</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>129</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G14" s="13">
         <v>2</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K14" s="50"/>
       <c r="L14" s="77">
@@ -2677,7 +2675,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>136</v>
@@ -2701,7 +2699,7 @@
         <v>134</v>
       </c>
       <c r="K15" s="51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L15" s="11">
         <v>0.64890000000000003</v>
@@ -2720,7 +2718,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>137</v>
@@ -2744,7 +2742,7 @@
         <v>132</v>
       </c>
       <c r="K16" s="51" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L16" s="11">
         <v>1.2175</v>
@@ -2763,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>150</v>
@@ -2787,7 +2785,7 @@
         <v>152</v>
       </c>
       <c r="K17" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L17" s="11">
         <v>4.8</v>
@@ -2806,7 +2804,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>144</v>
@@ -2830,7 +2828,7 @@
         <v>142</v>
       </c>
       <c r="K18" s="50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L18" s="19">
         <v>3.2381700000000002</v>
@@ -2849,7 +2847,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>13</v>
@@ -2892,7 +2890,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>12</v>
@@ -2935,29 +2933,29 @@
         <v>2</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>74</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G21" s="13">
         <v>2</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K21" s="50"/>
-      <c r="L21" s="77">
+      <c r="L21" s="91">
         <v>2.3774600000000001</v>
       </c>
       <c r="M21" s="85">
@@ -2967,54 +2965,50 @@
     </row>
     <row r="22" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
-        <f t="shared" si="0"/>
+        <f>A21+1</f>
         <v>16</v>
       </c>
-      <c r="B22" s="25">
-        <v>75</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>338</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>256</v>
+      <c r="B22" s="78">
+        <v>2</v>
+      </c>
+      <c r="C22" s="83" t="s">
+        <v>417</v>
+      </c>
+      <c r="D22" s="66" t="s">
+        <v>419</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="F22" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" s="81" t="s">
         <v>53</v>
       </c>
       <c r="G22" s="13">
         <v>2</v>
       </c>
-      <c r="H22" s="14" t="s">
-        <v>257</v>
-      </c>
+      <c r="H22" s="14"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="10" t="s">
-        <v>258</v>
-      </c>
+      <c r="J22" s="10"/>
       <c r="K22" s="50"/>
-      <c r="L22" s="19"/>
+      <c r="L22" s="77"/>
       <c r="M22" s="85"/>
     </row>
     <row r="23" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A23:A86" si="2">A22+1</f>
         <v>17</v>
       </c>
       <c r="B23" s="25">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>339</v>
-      </c>
-      <c r="D23" s="55" t="s">
-        <v>283</v>
+        <v>337</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>255</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="F23" s="20" t="s">
         <v>53</v>
@@ -3023,11 +3017,11 @@
         <v>2</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>284</v>
+        <v>256</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10" t="s">
-        <v>285</v>
+        <v>257</v>
       </c>
       <c r="K23" s="50"/>
       <c r="L23" s="19"/>
@@ -3035,542 +3029,539 @@
     </row>
     <row r="24" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="B24" s="78">
-        <v>25</v>
-      </c>
-      <c r="C24" s="63" t="s">
-        <v>340</v>
+      <c r="B24" s="25">
+        <v>40</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>338</v>
       </c>
       <c r="D24" s="55" t="s">
-        <v>250</v>
+        <v>282</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" s="20"/>
+        <v>125</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>53</v>
+      </c>
       <c r="G24" s="13">
         <v>2</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>251</v>
+        <v>283</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="s">
-        <v>249</v>
+        <v>284</v>
       </c>
       <c r="K24" s="50"/>
-      <c r="L24" s="19">
-        <v>7.2650000000000006E-2</v>
-      </c>
-      <c r="M24" s="85">
-        <f t="shared" ref="M24:M31" si="2">B24*L24</f>
-        <v>1.8162500000000001</v>
-      </c>
+      <c r="L24" s="19"/>
+      <c r="M24" s="85"/>
     </row>
     <row r="25" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="B25" s="25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>120</v>
+      <c r="B25" s="78">
+        <v>25</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>339</v>
       </c>
       <c r="D25" s="55" t="s">
-        <v>298</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>121</v>
+        <v>249</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="13">
         <v>2</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>297</v>
+        <v>250</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10" t="s">
-        <v>299</v>
+        <v>248</v>
       </c>
       <c r="K25" s="50"/>
       <c r="L25" s="19">
-        <v>0.41160000000000002</v>
+        <v>7.2650000000000006E-2</v>
       </c>
       <c r="M25" s="85">
-        <f t="shared" si="2"/>
-        <v>0.41160000000000002</v>
+        <f t="shared" ref="M25:M32" si="3">B25*L25</f>
+        <v>1.8162500000000001</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="B26" s="78">
-        <v>3</v>
-      </c>
-      <c r="C26" s="63" t="s">
-        <v>341</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="55" t="s">
-        <v>301</v>
-      </c>
+      <c r="B26" s="25">
+        <v>1</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="55" t="s">
+        <v>297</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="20"/>
       <c r="G26" s="13">
         <v>2</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="K26" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="L26" s="77">
-        <v>0.31574999999999998</v>
+        <v>296</v>
+      </c>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="K26" s="50"/>
+      <c r="L26" s="19">
+        <v>0.41160000000000002</v>
       </c>
       <c r="M26" s="85">
-        <f t="shared" si="2"/>
-        <v>0.94724999999999993</v>
+        <f t="shared" si="3"/>
+        <v>0.41160000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="B27" s="78">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>80</v>
+        <v>18</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="55" t="s">
+        <v>300</v>
       </c>
       <c r="G27" s="13">
         <v>2</v>
       </c>
-      <c r="H27" s="16" t="s">
-        <v>111</v>
+      <c r="H27" s="14" t="s">
+        <v>299</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J27" s="10" t="s">
-        <v>112</v>
+      <c r="J27" s="14" t="s">
+        <v>301</v>
       </c>
       <c r="K27" s="51" t="s">
-        <v>181</v>
-      </c>
-      <c r="L27" s="19">
-        <v>4.31034482758621E-2</v>
+        <v>90</v>
+      </c>
+      <c r="L27" s="77">
+        <v>0.31574999999999998</v>
       </c>
       <c r="M27" s="85">
-        <f t="shared" si="2"/>
-        <v>0.3448275862068968</v>
+        <f t="shared" si="3"/>
+        <v>0.94724999999999993</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="B28" s="25">
-        <v>2</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" s="49">
-        <v>2</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>82</v>
+      <c r="B28" s="78">
+        <v>8</v>
+      </c>
+      <c r="C28" s="63" t="s">
+        <v>341</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="13">
+        <v>2</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>111</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="K28" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="L28" s="11">
-        <v>5.72</v>
+        <v>52</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="K28" s="51" t="s">
+        <v>181</v>
+      </c>
+      <c r="L28" s="19">
+        <v>4.31034482758621E-2</v>
       </c>
       <c r="M28" s="85">
-        <f t="shared" si="2"/>
-        <v>11.44</v>
+        <f t="shared" si="3"/>
+        <v>0.3448275862068968</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="B29" s="25">
         <v>2</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="37" t="s">
-        <v>402</v>
+        <v>56</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="49">
+        <v>2</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K29" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="L29" s="19">
-        <v>3.3448000000000002</v>
+        <v>70</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K29" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="L29" s="11">
+        <v>5.72</v>
       </c>
       <c r="M29" s="85">
-        <f t="shared" si="2"/>
-        <v>6.6896000000000004</v>
+        <f t="shared" si="3"/>
+        <v>11.44</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B30" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="D30" s="55" t="s">
-        <v>212</v>
-      </c>
-      <c r="E30" s="55" t="s">
-        <v>210</v>
+        <v>57</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>58</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>303</v>
+        <v>16</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>11</v>
+        <v>400</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="I30" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="J30" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="K30" s="50"/>
-      <c r="L30" s="77">
-        <v>2.1168</v>
+        <v>14</v>
+      </c>
+      <c r="K30" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="L30" s="19">
+        <v>3.3448000000000002</v>
       </c>
       <c r="M30" s="85">
-        <f t="shared" si="2"/>
-        <v>2.1168</v>
+        <f t="shared" si="3"/>
+        <v>6.6896000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="B31" s="25">
         <v>1</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="13">
-        <v>2</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>52</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="D31" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>209</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K31" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="L31" s="19">
-        <v>0.09</v>
+        <v>208</v>
+      </c>
+      <c r="K31" s="50"/>
+      <c r="L31" s="77">
+        <v>2.1168</v>
       </c>
       <c r="M31" s="85">
-        <f t="shared" si="2"/>
-        <v>0.09</v>
+        <f t="shared" si="3"/>
+        <v>2.1168</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="B32" s="25">
         <v>1</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>312</v>
-      </c>
-      <c r="D32" s="55" t="s">
-        <v>377</v>
+        <v>310</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>378</v>
+        <v>399</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="G32" s="13">
         <v>2</v>
       </c>
-      <c r="H32" s="51" t="s">
-        <v>379</v>
-      </c>
-      <c r="I32" s="55" t="s">
+      <c r="H32" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J32" s="80" t="s">
-        <v>380</v>
+      <c r="J32" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="K32" s="51" t="s">
-        <v>381</v>
-      </c>
-      <c r="L32" s="19"/>
-      <c r="M32" s="85"/>
+        <v>37</v>
+      </c>
+      <c r="L32" s="19">
+        <v>0.09</v>
+      </c>
+      <c r="M32" s="85">
+        <f t="shared" si="3"/>
+        <v>0.09</v>
+      </c>
     </row>
     <row r="33" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="B33" s="25">
         <v>1</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="D33" s="66" t="s">
-        <v>405</v>
-      </c>
-      <c r="E33" s="66" t="s">
-        <v>71</v>
-      </c>
-      <c r="F33" s="81" t="s">
-        <v>382</v>
-      </c>
-      <c r="G33" s="37"/>
-      <c r="H33" s="80" t="s">
-        <v>383</v>
+        <v>311</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>376</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>377</v>
+      </c>
+      <c r="G33" s="13">
+        <v>2</v>
+      </c>
+      <c r="H33" s="51" t="s">
+        <v>378</v>
       </c>
       <c r="I33" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="J33" s="66" t="s">
-        <v>384</v>
-      </c>
-      <c r="K33" s="80"/>
-      <c r="L33" s="82">
-        <v>11.4</v>
-      </c>
-      <c r="M33" s="85">
-        <f t="shared" ref="M33:M48" si="3">B33*L33</f>
-        <v>11.4</v>
-      </c>
+      <c r="J33" s="80" t="s">
+        <v>379</v>
+      </c>
+      <c r="K33" s="51" t="s">
+        <v>380</v>
+      </c>
+      <c r="L33" s="19"/>
+      <c r="M33" s="85"/>
     </row>
     <row r="34" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="B34" s="25">
         <v>1</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D34" s="66" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="E34" s="66" t="s">
-        <v>388</v>
+        <v>71</v>
       </c>
       <c r="F34" s="81" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="G34" s="37"/>
       <c r="H34" s="80" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="I34" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J34" s="66" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="K34" s="80"/>
       <c r="L34" s="82">
-        <v>0.43</v>
+        <v>11.4</v>
       </c>
       <c r="M34" s="85">
-        <f t="shared" si="3"/>
-        <v>0.43</v>
+        <f t="shared" ref="M34:M48" si="4">B34*L34</f>
+        <v>11.4</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="B35" s="25">
         <v>1</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>313</v>
+        <v>343</v>
       </c>
       <c r="D35" s="66" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="E35" s="66" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="F35" s="81" t="s">
-        <v>396</v>
-      </c>
-      <c r="G35" s="13">
-        <v>2</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="G35" s="37"/>
       <c r="H35" s="80" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="I35" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J35" s="66" t="s">
-        <v>394</v>
-      </c>
-      <c r="K35" s="80" t="s">
-        <v>397</v>
-      </c>
-      <c r="L35" s="82"/>
+        <v>384</v>
+      </c>
+      <c r="K35" s="80"/>
+      <c r="L35" s="82">
+        <v>0.43</v>
+      </c>
       <c r="M35" s="85">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>0.43</v>
       </c>
     </row>
     <row r="36" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B36" s="25">
         <v>1</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="55" t="s">
-        <v>290</v>
+        <v>312</v>
+      </c>
+      <c r="D36" s="66" t="s">
+        <v>396</v>
       </c>
       <c r="E36" s="66" t="s">
-        <v>287</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="G36" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="50"/>
-      <c r="L36" s="19">
-        <v>2.2599999999999998</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="F36" s="81" t="s">
+        <v>394</v>
+      </c>
+      <c r="G36" s="13">
+        <v>2</v>
+      </c>
+      <c r="H36" s="80" t="s">
+        <v>393</v>
+      </c>
+      <c r="I36" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="J36" s="66" t="s">
+        <v>392</v>
+      </c>
+      <c r="K36" s="80" t="s">
+        <v>395</v>
+      </c>
+      <c r="L36" s="82"/>
       <c r="M36" s="85">
-        <f t="shared" si="3"/>
-        <v>2.2599999999999998</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="B37" s="25">
         <v>1</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>228</v>
+        <v>55</v>
       </c>
       <c r="D37" s="55" t="s">
         <v>289</v>
       </c>
-      <c r="E37" s="55" t="s">
-        <v>287</v>
+      <c r="E37" s="66" t="s">
+        <v>286</v>
       </c>
       <c r="F37" s="20" t="s">
         <v>135</v>
@@ -3579,7 +3570,7 @@
         <v>11</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
@@ -3588,26 +3579,26 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="M37" s="85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="B38" s="25">
         <v>1</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>156</v>
+        <v>227</v>
       </c>
       <c r="D38" s="55" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>230</v>
+        <v>286</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>135</v>
@@ -3616,35 +3607,35 @@
         <v>11</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
       <c r="K38" s="50"/>
       <c r="L38" s="19">
-        <v>1.79</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="M38" s="85">
-        <f t="shared" si="3"/>
-        <v>1.79</v>
+        <f t="shared" si="4"/>
+        <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="39" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B39" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D39" s="55" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F39" s="20" t="s">
         <v>135</v>
@@ -3653,34 +3644,34 @@
         <v>11</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
       <c r="K39" s="50"/>
       <c r="L39" s="19">
-        <v>1.34</v>
+        <v>1.79</v>
       </c>
       <c r="M39" s="85">
-        <f t="shared" si="3"/>
-        <v>2.68</v>
+        <f t="shared" si="4"/>
+        <v>1.79</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="B40" s="25">
         <v>2</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>345</v>
+        <v>157</v>
       </c>
       <c r="D40" s="55" t="s">
-        <v>294</v>
-      </c>
-      <c r="E40" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="E40" s="55" t="s">
         <v>229</v>
       </c>
       <c r="F40" s="20" t="s">
@@ -3690,141 +3681,148 @@
         <v>11</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
       <c r="K40" s="50"/>
       <c r="L40" s="19">
-        <v>0.26</v>
+        <v>1.34</v>
       </c>
       <c r="M40" s="85">
-        <f t="shared" si="3"/>
-        <v>0.52</v>
+        <f t="shared" si="4"/>
+        <v>2.68</v>
       </c>
     </row>
     <row r="41" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <f>A40+1</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="B41" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>417</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="G41" s="13">
-        <v>2</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="J41" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="K41" s="51"/>
+        <v>344</v>
+      </c>
+      <c r="D41" s="55" t="s">
+        <v>293</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="50"/>
       <c r="L41" s="19">
-        <v>3.5520000000000003E-2</v>
+        <v>0.26</v>
       </c>
       <c r="M41" s="85">
-        <f t="shared" si="3"/>
-        <v>3.5520000000000003E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.52</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
-        <f>A41+1</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="B42" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>418</v>
+        <v>306</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>51</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>419</v>
-      </c>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
+        <v>236</v>
+      </c>
+      <c r="G42" s="13">
+        <v>2</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>308</v>
+      </c>
       <c r="K42" s="51"/>
-      <c r="L42" s="77"/>
-      <c r="M42" s="85"/>
+      <c r="L42" s="19">
+        <v>3.5520000000000003E-2</v>
+      </c>
+      <c r="M42" s="85">
+        <f t="shared" si="4"/>
+        <v>3.5520000000000003E-2</v>
+      </c>
     </row>
     <row r="43" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
-        <f t="shared" ref="A43:A93" si="4">A42+1</f>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="B43" s="25">
         <v>4</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E43" s="64" t="s">
         <v>125</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G43" s="13">
         <v>2</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I43" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K43" s="51"/>
       <c r="L43" s="19">
         <v>2.8160000000000001E-2</v>
       </c>
       <c r="M43" s="85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.11264</v>
       </c>
     </row>
     <row r="44" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="B44" s="25">
         <v>2</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>155</v>
@@ -3854,13 +3852,13 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="M44" s="85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.114</v>
       </c>
     </row>
     <row r="45" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="B45" s="25">
@@ -3897,13 +3895,13 @@
         <v>1.40408</v>
       </c>
       <c r="M45" s="85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.80816</v>
       </c>
     </row>
     <row r="46" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="B46" s="25">
@@ -3940,35 +3938,35 @@
         <v>0.7</v>
       </c>
       <c r="M46" s="85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
     </row>
     <row r="47" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="B47" s="25">
         <v>2</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D47" s="55" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>108</v>
       </c>
       <c r="F47" s="67" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G47" s="68">
         <v>2</v>
       </c>
       <c r="H47" s="69" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I47" s="70"/>
       <c r="J47" s="71"/>
@@ -3979,20 +3977,20 @@
         <v>6.6299999999999998E-2</v>
       </c>
       <c r="M47" s="85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.1326</v>
       </c>
     </row>
     <row r="48" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="B48" s="25">
         <v>1</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>116</v>
@@ -4022,23 +4020,23 @@
         <v>0.34899999999999998</v>
       </c>
       <c r="M48" s="85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.34899999999999998</v>
       </c>
     </row>
     <row r="49" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="B49" s="25">
         <v>8</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D49" s="55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E49" s="64" t="s">
         <v>176</v>
@@ -4058,17 +4056,17 @@
     </row>
     <row r="50" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="B50" s="25">
         <v>1</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E50" s="64" t="s">
         <v>125</v>
@@ -4088,17 +4086,17 @@
     </row>
     <row r="51" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="B51" s="25">
         <v>23</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E51" s="64" t="s">
         <v>125</v>
@@ -4118,17 +4116,17 @@
     </row>
     <row r="52" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="B52" s="25">
         <v>3</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E52" s="64" t="s">
         <v>125</v>
@@ -4148,17 +4146,17 @@
     </row>
     <row r="53" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="B53" s="25">
         <v>4</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E53" s="64" t="s">
         <v>125</v>
@@ -4178,17 +4176,17 @@
     </row>
     <row r="54" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="B54" s="25">
         <v>6</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E54" s="64" t="s">
         <v>125</v>
@@ -4208,17 +4206,17 @@
     </row>
     <row r="55" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="B55" s="79">
         <v>10</v>
       </c>
       <c r="C55" s="83" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E55" s="64" t="s">
         <v>125</v>
@@ -4238,17 +4236,17 @@
     </row>
     <row r="56" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="B56" s="79">
         <v>5</v>
       </c>
       <c r="C56" s="83" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E56" s="64" t="s">
         <v>125</v>
@@ -4268,14 +4266,14 @@
     </row>
     <row r="57" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="B57" s="79">
         <v>0</v>
       </c>
       <c r="C57" s="83" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D57" s="55" t="s">
         <v>0</v>
@@ -4296,17 +4294,17 @@
     </row>
     <row r="58" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="B58" s="79">
         <v>4</v>
       </c>
       <c r="C58" s="83" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E58" s="64" t="s">
         <v>125</v>
@@ -4326,17 +4324,17 @@
     </row>
     <row r="59" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
       <c r="B59" s="25">
         <v>2</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E59" s="64" t="s">
         <v>125</v>
@@ -4356,17 +4354,17 @@
     </row>
     <row r="60" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="B60" s="78">
         <v>11</v>
       </c>
       <c r="C60" s="63" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E60" s="64" t="s">
         <v>125</v>
@@ -4386,17 +4384,17 @@
     </row>
     <row r="61" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="B61" s="78">
         <v>2</v>
       </c>
       <c r="C61" s="63" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E61" s="64" t="s">
         <v>125</v>
@@ -4416,17 +4414,17 @@
     </row>
     <row r="62" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
       <c r="B62" s="25">
         <v>2</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E62" s="64" t="s">
         <v>125</v>
@@ -4446,17 +4444,17 @@
     </row>
     <row r="63" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="B63" s="25">
         <v>11</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E63" s="64" t="s">
         <v>125</v>
@@ -4476,17 +4474,17 @@
     </row>
     <row r="64" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="B64" s="25">
         <v>1</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E64" s="64" t="s">
         <v>125</v>
@@ -4506,17 +4504,17 @@
     </row>
     <row r="65" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="B65" s="25">
         <v>1</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D65" s="66" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E65" s="64" t="s">
         <v>125</v>
@@ -4536,17 +4534,17 @@
     </row>
     <row r="66" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="B66" s="25">
         <v>2</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D66" s="66" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E66" s="64" t="s">
         <v>125</v>
@@ -4566,17 +4564,17 @@
     </row>
     <row r="67" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="B67" s="25">
         <v>1</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E67" s="64" t="s">
         <v>125</v>
@@ -4586,11 +4584,11 @@
         <v>2</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I67" s="10"/>
       <c r="J67" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K67" s="50"/>
       <c r="L67" s="19">
@@ -4603,17 +4601,17 @@
     </row>
     <row r="68" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="B68" s="25">
         <v>7</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E68" s="64" t="s">
         <v>125</v>
@@ -4623,11 +4621,11 @@
         <v>2</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I68" s="10"/>
       <c r="J68" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K68" s="50"/>
       <c r="L68" s="19">
@@ -4640,17 +4638,17 @@
     </row>
     <row r="69" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="B69" s="25">
         <v>1</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E69" s="64" t="s">
         <v>125</v>
@@ -4660,11 +4658,11 @@
         <v>2</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I69" s="10"/>
       <c r="J69" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K69" s="51"/>
       <c r="L69" s="19">
@@ -4677,17 +4675,17 @@
     </row>
     <row r="70" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="B70" s="25">
         <v>2</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E70" s="64" t="s">
         <v>125</v>
@@ -4697,11 +4695,11 @@
         <v>2</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I70" s="10"/>
       <c r="J70" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K70" s="50"/>
       <c r="L70" s="19">
@@ -4714,17 +4712,17 @@
     </row>
     <row r="71" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="B71" s="25">
         <v>1</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D71" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E71" s="64" t="s">
         <v>125</v>
@@ -4734,11 +4732,11 @@
         <v>2</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I71" s="10"/>
       <c r="J71" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K71" s="50"/>
       <c r="L71" s="77">
@@ -4751,14 +4749,14 @@
     </row>
     <row r="72" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="B72" s="25">
         <v>8</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D72" s="20" t="s">
         <v>97</v>
@@ -4794,17 +4792,17 @@
     </row>
     <row r="73" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="B73" s="25">
         <v>2</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E73" s="21" t="s">
         <v>69</v>
@@ -4814,13 +4812,13 @@
         <v>2</v>
       </c>
       <c r="H73" s="10" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I73" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="K73" s="51"/>
       <c r="L73" s="19">
@@ -4833,7 +4831,7 @@
     </row>
     <row r="74" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="B74" s="25">
@@ -4876,7 +4874,7 @@
     </row>
     <row r="75" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="B75" s="25">
@@ -4919,7 +4917,7 @@
     </row>
     <row r="76" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="B76" s="25">
@@ -4929,7 +4927,7 @@
         <v>50</v>
       </c>
       <c r="D76" s="55" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>159</v>
@@ -4939,13 +4937,13 @@
       </c>
       <c r="G76" s="37"/>
       <c r="H76" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I76" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J76" s="62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K76" s="62"/>
       <c r="L76" s="19">
@@ -4958,7 +4956,7 @@
     </row>
     <row r="77" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="B77" s="25">
@@ -4968,7 +4966,7 @@
         <v>160</v>
       </c>
       <c r="D77" s="55" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>161</v>
@@ -4999,7 +4997,7 @@
     </row>
     <row r="78" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="B78" s="25">
@@ -5009,23 +5007,23 @@
         <v>122</v>
       </c>
       <c r="D78" s="55" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>162</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G78" s="37" t="s">
         <v>11</v>
       </c>
       <c r="H78" s="51" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I78" s="10"/>
       <c r="J78" s="51" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K78" s="62"/>
       <c r="L78" s="77">
@@ -5038,7 +5036,7 @@
     </row>
     <row r="79" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="B79" s="25">
@@ -5079,7 +5077,7 @@
     </row>
     <row r="80" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="B80" s="25">
@@ -5120,7 +5118,7 @@
     </row>
     <row r="81" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="B81" s="25">
@@ -5163,7 +5161,7 @@
     </row>
     <row r="82" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="B82" s="25">
@@ -5173,7 +5171,7 @@
         <v>165</v>
       </c>
       <c r="D82" s="55" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>108</v>
@@ -5185,13 +5183,13 @@
         <v>2</v>
       </c>
       <c r="H82" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I82" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K82" s="62"/>
       <c r="L82" s="19">
@@ -5204,7 +5202,7 @@
     </row>
     <row r="83" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="B83" s="25">
@@ -5214,25 +5212,25 @@
         <v>166</v>
       </c>
       <c r="D83" s="55" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>108</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G83" s="13">
         <v>2</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I83" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K83" s="62"/>
       <c r="L83" s="77">
@@ -5245,14 +5243,14 @@
     </row>
     <row r="84" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="B84" s="25">
         <v>2</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D84" s="10" t="s">
         <v>196</v>
@@ -5280,14 +5278,14 @@
     </row>
     <row r="85" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
       <c r="B85" s="25">
         <v>2</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D85" s="20" t="s">
         <v>28</v>
@@ -5323,14 +5321,14 @@
     </row>
     <row r="86" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="B86" s="25">
         <v>1</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D86" s="10" t="s">
         <v>126</v>
@@ -5366,14 +5364,14 @@
     </row>
     <row r="87" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A87:A93" si="6">A86+1</f>
         <v>81</v>
       </c>
       <c r="B87" s="25">
         <v>1</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D87" s="10" t="s">
         <v>197</v>
@@ -5407,17 +5405,17 @@
     </row>
     <row r="88" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>82</v>
       </c>
       <c r="B88" s="25">
         <v>1</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>198</v>
+        <v>418</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>172</v>
@@ -5448,7 +5446,7 @@
     </row>
     <row r="89" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>83</v>
       </c>
       <c r="B89" s="25">
@@ -5458,7 +5456,7 @@
         <v>168</v>
       </c>
       <c r="D89" s="55" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>174</v>
@@ -5470,11 +5468,11 @@
         <v>1</v>
       </c>
       <c r="H89" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I89" s="10"/>
       <c r="J89" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K89" s="62"/>
       <c r="L89" s="77">
@@ -5487,7 +5485,7 @@
     </row>
     <row r="90" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>84</v>
       </c>
       <c r="B90" s="25">
@@ -5497,7 +5495,7 @@
         <v>169</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E90" s="10" t="s">
         <v>61</v>
@@ -5526,7 +5524,7 @@
     </row>
     <row r="91" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>85</v>
       </c>
       <c r="B91" s="25">
@@ -5536,25 +5534,25 @@
         <v>171</v>
       </c>
       <c r="D91" s="66" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E91" s="15" t="s">
         <v>123</v>
       </c>
       <c r="F91" s="66" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G91" s="13">
         <v>2</v>
       </c>
       <c r="H91" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I91" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J91" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K91" s="60" t="s">
         <v>180</v>
@@ -5569,7 +5567,7 @@
     </row>
     <row r="92" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>86</v>
       </c>
       <c r="B92" s="25">
@@ -5579,23 +5577,23 @@
         <v>173</v>
       </c>
       <c r="D92" s="66" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>123</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G92" s="13">
         <v>2</v>
       </c>
       <c r="H92" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I92" s="10"/>
       <c r="J92" s="55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K92" s="50"/>
       <c r="L92" s="77">
@@ -5608,7 +5606,7 @@
     </row>
     <row r="93" spans="1:13" s="24" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>87</v>
       </c>
       <c r="B93" s="29">
@@ -5616,7 +5614,7 @@
       </c>
       <c r="C93" s="30"/>
       <c r="D93" s="73" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E93" s="32"/>
       <c r="F93" s="31"/>
@@ -5675,7 +5673,7 @@
         <v>94</v>
       </c>
       <c r="C99" s="76" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D99" s="72"/>
       <c r="E99" s="72"/>
@@ -5765,7 +5763,7 @@
         <v>3</v>
       </c>
       <c r="C106" s="56" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
@@ -5773,7 +5771,7 @@
         <v>4</v>
       </c>
       <c r="C107" s="75" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
@@ -5781,7 +5779,7 @@
         <v>5</v>
       </c>
       <c r="C108" s="75" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update P/N for Xilinx FPGA to allow -2 or -3 speed grade and any temperature grade
</commit_message>
<xml_diff>
--- a/FPGA1394V3-BOM.xlsx
+++ b/FPGA1394V3-BOM.xlsx
@@ -710,12 +710,6 @@
     <t>IC, DDR Termination Power Supply, LP2998</t>
   </si>
   <si>
-    <t>XC7Z020-3CLG400E</t>
-  </si>
-  <si>
-    <t>122-2186-ND</t>
-  </si>
-  <si>
     <t>Winbond</t>
   </si>
   <si>
@@ -1481,9 +1475,6 @@
     <t>L8</t>
   </si>
   <si>
-    <t>L9-10 have been replaced by 0 Ohm resistors</t>
-  </si>
-  <si>
     <t>IEEE-1394/Ethernet FPGA Board, Rev 3.2</t>
   </si>
   <si>
@@ -1494,6 +1485,15 @@
   </si>
   <si>
     <t>CAP, 4700pF, 10%, 16V, X7R, 0402</t>
+  </si>
+  <si>
+    <t>XC7Z020-sCLG400t</t>
+  </si>
+  <si>
+    <t>122-1848-ND</t>
+  </si>
+  <si>
+    <t>XC7Z020-sCLG400t, where s (speed grade) can be 2 or 3 and t (temperature grade) can be C, I or E</t>
   </si>
 </sst>
 </file>
@@ -1925,13 +1925,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2241,8 +2241,8 @@
   </sheetPr>
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2265,7 +2265,7 @@
     <row r="1" spans="1:13" ht="29.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2280,7 +2280,7 @@
     <row r="2" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2295,7 +2295,7 @@
     <row r="3" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="22">
-        <v>45569</v>
+        <v>45575</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2389,7 +2389,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>175</v>
@@ -2419,7 +2419,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>6</v>
@@ -2462,10 +2462,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>125</v>
@@ -2492,10 +2492,10 @@
         <v>21</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>125</v>
@@ -2524,10 +2524,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D11" s="55" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>125</v>
@@ -2539,11 +2539,11 @@
         <v>2</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K11" s="50"/>
       <c r="L11" s="19"/>
@@ -2558,26 +2558,26 @@
         <v>5</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D12" s="55" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>54</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G12" s="13">
         <v>2</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="K12" s="50"/>
       <c r="L12" s="77">
@@ -2597,26 +2597,26 @@
         <v>13</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G13" s="13">
         <v>2</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K13" s="50"/>
       <c r="L13" s="19">
@@ -2636,26 +2636,26 @@
         <v>2</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>129</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G14" s="13">
         <v>2</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K14" s="50"/>
       <c r="L14" s="77">
@@ -2675,7 +2675,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>136</v>
@@ -2699,7 +2699,7 @@
         <v>134</v>
       </c>
       <c r="K15" s="51" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L15" s="11">
         <v>0.64890000000000003</v>
@@ -2718,7 +2718,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>137</v>
@@ -2742,7 +2742,7 @@
         <v>132</v>
       </c>
       <c r="K16" s="51" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L16" s="11">
         <v>1.2175</v>
@@ -2761,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>150</v>
@@ -2785,7 +2785,7 @@
         <v>152</v>
       </c>
       <c r="K17" s="50" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L17" s="11">
         <v>4.8</v>
@@ -2804,7 +2804,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>144</v>
@@ -2828,7 +2828,7 @@
         <v>142</v>
       </c>
       <c r="K18" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L18" s="19">
         <v>3.2381700000000002</v>
@@ -2847,7 +2847,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>13</v>
@@ -2890,7 +2890,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>12</v>
@@ -2933,29 +2933,29 @@
         <v>2</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>74</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G21" s="13">
         <v>2</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K21" s="50"/>
-      <c r="L21" s="91">
+      <c r="L21" s="87">
         <v>2.3774600000000001</v>
       </c>
       <c r="M21" s="85">
@@ -2972,10 +2972,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="83" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D22" s="66" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>125</v>
@@ -3002,10 +3002,10 @@
         <v>75</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>176</v>
@@ -3017,11 +3017,11 @@
         <v>2</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K23" s="50"/>
       <c r="L23" s="19"/>
@@ -3036,10 +3036,10 @@
         <v>40</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D24" s="55" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>125</v>
@@ -3051,11 +3051,11 @@
         <v>2</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K24" s="50"/>
       <c r="L24" s="19"/>
@@ -3070,10 +3070,10 @@
         <v>25</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D25" s="55" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>51</v>
@@ -3083,11 +3083,11 @@
         <v>2</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K25" s="50"/>
       <c r="L25" s="19">
@@ -3110,7 +3110,7 @@
         <v>120</v>
       </c>
       <c r="D26" s="55" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>121</v>
@@ -3120,11 +3120,11 @@
         <v>2</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K26" s="50"/>
       <c r="L26" s="19">
@@ -3144,7 +3144,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>18</v>
@@ -3153,19 +3153,19 @@
         <v>54</v>
       </c>
       <c r="F27" s="55" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G27" s="13">
         <v>2</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K27" s="51" t="s">
         <v>90</v>
@@ -3187,7 +3187,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>113</v>
@@ -3285,7 +3285,7 @@
         <v>16</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H30" s="14" t="s">
         <v>15</v>
@@ -3316,26 +3316,26 @@
         <v>1</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D31" s="55" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G31" s="37" t="s">
         <v>11</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K31" s="50"/>
       <c r="L31" s="77">
@@ -3355,13 +3355,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>1</v>
@@ -3398,31 +3398,31 @@
         <v>1</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D33" s="55" t="s">
+        <v>374</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="G33" s="13">
+        <v>2</v>
+      </c>
+      <c r="H33" s="51" t="s">
         <v>376</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>377</v>
-      </c>
-      <c r="G33" s="13">
-        <v>2</v>
-      </c>
-      <c r="H33" s="51" t="s">
-        <v>378</v>
       </c>
       <c r="I33" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J33" s="80" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="K33" s="51" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="85"/>
@@ -3436,26 +3436,26 @@
         <v>1</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D34" s="66" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E34" s="66" t="s">
         <v>71</v>
       </c>
       <c r="F34" s="81" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G34" s="37"/>
       <c r="H34" s="80" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I34" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J34" s="66" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K34" s="80"/>
       <c r="L34" s="82">
@@ -3475,26 +3475,26 @@
         <v>1</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D35" s="66" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E35" s="66" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F35" s="81" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G35" s="37"/>
       <c r="H35" s="80" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I35" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J35" s="66" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K35" s="80"/>
       <c r="L35" s="82">
@@ -3514,31 +3514,31 @@
         <v>1</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D36" s="66" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E36" s="66" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F36" s="81" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G36" s="13">
         <v>2</v>
       </c>
       <c r="H36" s="80" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I36" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J36" s="66" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K36" s="80" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L36" s="82"/>
       <c r="M36" s="85">
@@ -3558,10 +3558,10 @@
         <v>55</v>
       </c>
       <c r="D37" s="55" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E37" s="66" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F37" s="20" t="s">
         <v>135</v>
@@ -3570,7 +3570,7 @@
         <v>11</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
@@ -3592,13 +3592,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D38" s="55" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>135</v>
@@ -3607,7 +3607,7 @@
         <v>11</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
@@ -3632,10 +3632,10 @@
         <v>156</v>
       </c>
       <c r="D39" s="55" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F39" s="20" t="s">
         <v>135</v>
@@ -3644,7 +3644,7 @@
         <v>11</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
@@ -3669,10 +3669,10 @@
         <v>157</v>
       </c>
       <c r="D40" s="55" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F40" s="20" t="s">
         <v>135</v>
@@ -3681,7 +3681,7 @@
         <v>11</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
@@ -3703,13 +3703,13 @@
         <v>2</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D41" s="55" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F41" s="20" t="s">
         <v>135</v>
@@ -3718,7 +3718,7 @@
         <v>11</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
@@ -3740,28 +3740,28 @@
         <v>1</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>51</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G42" s="13">
         <v>2</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I42" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K42" s="51"/>
       <c r="L42" s="19">
@@ -3781,28 +3781,28 @@
         <v>4</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E43" s="64" t="s">
         <v>125</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G43" s="13">
         <v>2</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I43" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K43" s="51"/>
       <c r="L43" s="19">
@@ -3822,7 +3822,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>155</v>
@@ -3951,22 +3951,22 @@
         <v>2</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D47" s="55" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>108</v>
       </c>
       <c r="F47" s="67" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G47" s="68">
         <v>2</v>
       </c>
       <c r="H47" s="69" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I47" s="70"/>
       <c r="J47" s="71"/>
@@ -3990,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>116</v>
@@ -4033,10 +4033,10 @@
         <v>8</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D49" s="55" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E49" s="64" t="s">
         <v>176</v>
@@ -4063,10 +4063,10 @@
         <v>1</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E50" s="64" t="s">
         <v>125</v>
@@ -4093,10 +4093,10 @@
         <v>23</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E51" s="64" t="s">
         <v>125</v>
@@ -4123,10 +4123,10 @@
         <v>3</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E52" s="64" t="s">
         <v>125</v>
@@ -4153,10 +4153,10 @@
         <v>4</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E53" s="64" t="s">
         <v>125</v>
@@ -4183,10 +4183,10 @@
         <v>6</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E54" s="64" t="s">
         <v>125</v>
@@ -4213,10 +4213,10 @@
         <v>10</v>
       </c>
       <c r="C55" s="83" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E55" s="64" t="s">
         <v>125</v>
@@ -4243,10 +4243,10 @@
         <v>5</v>
       </c>
       <c r="C56" s="83" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E56" s="64" t="s">
         <v>125</v>
@@ -4273,7 +4273,7 @@
         <v>0</v>
       </c>
       <c r="C57" s="83" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D57" s="55" t="s">
         <v>0</v>
@@ -4301,10 +4301,10 @@
         <v>4</v>
       </c>
       <c r="C58" s="83" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E58" s="64" t="s">
         <v>125</v>
@@ -4331,10 +4331,10 @@
         <v>2</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E59" s="64" t="s">
         <v>125</v>
@@ -4361,10 +4361,10 @@
         <v>11</v>
       </c>
       <c r="C60" s="63" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E60" s="64" t="s">
         <v>125</v>
@@ -4391,10 +4391,10 @@
         <v>2</v>
       </c>
       <c r="C61" s="63" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E61" s="64" t="s">
         <v>125</v>
@@ -4421,10 +4421,10 @@
         <v>2</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E62" s="64" t="s">
         <v>125</v>
@@ -4451,10 +4451,10 @@
         <v>11</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E63" s="64" t="s">
         <v>125</v>
@@ -4481,10 +4481,10 @@
         <v>1</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E64" s="64" t="s">
         <v>125</v>
@@ -4511,10 +4511,10 @@
         <v>1</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D65" s="66" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E65" s="64" t="s">
         <v>125</v>
@@ -4541,10 +4541,10 @@
         <v>2</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D66" s="66" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E66" s="64" t="s">
         <v>125</v>
@@ -4571,10 +4571,10 @@
         <v>1</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E67" s="64" t="s">
         <v>125</v>
@@ -4584,11 +4584,11 @@
         <v>2</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I67" s="10"/>
       <c r="J67" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K67" s="50"/>
       <c r="L67" s="19">
@@ -4608,10 +4608,10 @@
         <v>7</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E68" s="64" t="s">
         <v>125</v>
@@ -4621,11 +4621,11 @@
         <v>2</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I68" s="10"/>
       <c r="J68" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K68" s="50"/>
       <c r="L68" s="19">
@@ -4645,10 +4645,10 @@
         <v>1</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E69" s="64" t="s">
         <v>125</v>
@@ -4658,11 +4658,11 @@
         <v>2</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I69" s="10"/>
       <c r="J69" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K69" s="51"/>
       <c r="L69" s="19">
@@ -4682,10 +4682,10 @@
         <v>2</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E70" s="64" t="s">
         <v>125</v>
@@ -4695,11 +4695,11 @@
         <v>2</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I70" s="10"/>
       <c r="J70" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K70" s="50"/>
       <c r="L70" s="19">
@@ -4719,10 +4719,10 @@
         <v>1</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D71" s="20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E71" s="64" t="s">
         <v>125</v>
@@ -4732,11 +4732,11 @@
         <v>2</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I71" s="10"/>
       <c r="J71" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K71" s="50"/>
       <c r="L71" s="77">
@@ -4756,7 +4756,7 @@
         <v>8</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D72" s="20" t="s">
         <v>97</v>
@@ -4799,10 +4799,10 @@
         <v>2</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E73" s="21" t="s">
         <v>69</v>
@@ -4812,13 +4812,13 @@
         <v>2</v>
       </c>
       <c r="H73" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I73" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="K73" s="51"/>
       <c r="L73" s="19">
@@ -4927,7 +4927,7 @@
         <v>50</v>
       </c>
       <c r="D76" s="55" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>159</v>
@@ -4935,23 +4935,25 @@
       <c r="F76" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="G76" s="37"/>
-      <c r="H76" s="10" t="s">
-        <v>199</v>
+      <c r="G76" s="13">
+        <v>5</v>
+      </c>
+      <c r="H76" s="66" t="s">
+        <v>417</v>
       </c>
       <c r="I76" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J76" s="62" t="s">
-        <v>200</v>
+        <v>418</v>
       </c>
       <c r="K76" s="62"/>
       <c r="L76" s="19">
-        <v>198</v>
+        <v>180.7</v>
       </c>
       <c r="M76" s="85">
         <f t="shared" si="5"/>
-        <v>198</v>
+        <v>180.7</v>
       </c>
     </row>
     <row r="77" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -4966,7 +4968,7 @@
         <v>160</v>
       </c>
       <c r="D77" s="55" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>161</v>
@@ -5007,23 +5009,23 @@
         <v>122</v>
       </c>
       <c r="D78" s="55" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>162</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G78" s="37" t="s">
         <v>11</v>
       </c>
       <c r="H78" s="51" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I78" s="10"/>
       <c r="J78" s="51" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K78" s="62"/>
       <c r="L78" s="77">
@@ -5171,7 +5173,7 @@
         <v>165</v>
       </c>
       <c r="D82" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>108</v>
@@ -5183,13 +5185,13 @@
         <v>2</v>
       </c>
       <c r="H82" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I82" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K82" s="62"/>
       <c r="L82" s="19">
@@ -5212,25 +5214,25 @@
         <v>166</v>
       </c>
       <c r="D83" s="55" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>108</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G83" s="13">
         <v>2</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I83" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K83" s="62"/>
       <c r="L83" s="77">
@@ -5250,7 +5252,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D84" s="10" t="s">
         <v>196</v>
@@ -5285,7 +5287,7 @@
         <v>2</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D85" s="20" t="s">
         <v>28</v>
@@ -5328,7 +5330,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D86" s="10" t="s">
         <v>126</v>
@@ -5371,7 +5373,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D87" s="10" t="s">
         <v>197</v>
@@ -5412,10 +5414,10 @@
         <v>1</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>172</v>
@@ -5456,7 +5458,7 @@
         <v>168</v>
       </c>
       <c r="D89" s="55" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>174</v>
@@ -5468,11 +5470,11 @@
         <v>1</v>
       </c>
       <c r="H89" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I89" s="10"/>
       <c r="J89" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K89" s="62"/>
       <c r="L89" s="77">
@@ -5534,25 +5536,25 @@
         <v>171</v>
       </c>
       <c r="D91" s="66" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E91" s="15" t="s">
         <v>123</v>
       </c>
       <c r="F91" s="66" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G91" s="13">
         <v>2</v>
       </c>
       <c r="H91" s="10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I91" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J91" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K91" s="60" t="s">
         <v>180</v>
@@ -5577,23 +5579,23 @@
         <v>173</v>
       </c>
       <c r="D92" s="66" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>123</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G92" s="13">
         <v>2</v>
       </c>
       <c r="H92" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I92" s="10"/>
       <c r="J92" s="55" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K92" s="50"/>
       <c r="L92" s="77">
@@ -5614,7 +5616,7 @@
       </c>
       <c r="C93" s="30"/>
       <c r="D93" s="73" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E93" s="32"/>
       <c r="F93" s="31"/>
@@ -5641,7 +5643,7 @@
       </c>
       <c r="M94" s="36">
         <f>SUM(M7:M93)</f>
-        <v>384.95541758620681</v>
+        <v>367.65541758620685</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -5658,14 +5660,14 @@
       <c r="B98" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C98" s="87" t="s">
+      <c r="C98" s="88" t="s">
         <v>101</v>
       </c>
-      <c r="D98" s="87"/>
-      <c r="E98" s="87"/>
-      <c r="F98" s="87"/>
-      <c r="G98" s="87"/>
-      <c r="H98" s="87"/>
+      <c r="D98" s="88"/>
+      <c r="E98" s="88"/>
+      <c r="F98" s="88"/>
+      <c r="G98" s="88"/>
+      <c r="H98" s="88"/>
     </row>
     <row r="99" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="26"/>
@@ -5673,7 +5675,7 @@
         <v>94</v>
       </c>
       <c r="C99" s="76" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D99" s="72"/>
       <c r="E99" s="72"/>
@@ -5688,82 +5690,82 @@
       <c r="B100" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C100" s="88" t="s">
+      <c r="C100" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="D100" s="88"/>
-      <c r="E100" s="88"/>
-      <c r="F100" s="88"/>
-      <c r="G100" s="88"/>
-      <c r="H100" s="88"/>
+      <c r="D100" s="89"/>
+      <c r="E100" s="89"/>
+      <c r="F100" s="89"/>
+      <c r="G100" s="89"/>
+      <c r="H100" s="89"/>
     </row>
     <row r="101" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C101" s="89" t="s">
+      <c r="C101" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="D101" s="88"/>
-      <c r="E101" s="88"/>
-      <c r="F101" s="88"/>
-      <c r="G101" s="88"/>
-      <c r="H101" s="88"/>
+      <c r="D101" s="89"/>
+      <c r="E101" s="89"/>
+      <c r="F101" s="89"/>
+      <c r="G101" s="89"/>
+      <c r="H101" s="89"/>
     </row>
     <row r="102" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="9">
         <v>1</v>
       </c>
-      <c r="C102" s="88" t="s">
+      <c r="C102" s="89" t="s">
         <v>102</v>
       </c>
-      <c r="D102" s="88"/>
-      <c r="E102" s="88"/>
-      <c r="F102" s="88"/>
-      <c r="G102" s="88"/>
-      <c r="H102" s="88"/>
+      <c r="D102" s="89"/>
+      <c r="E102" s="89"/>
+      <c r="F102" s="89"/>
+      <c r="G102" s="89"/>
+      <c r="H102" s="89"/>
     </row>
     <row r="103" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="9"/>
-      <c r="C103" s="90" t="s">
+      <c r="C103" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="D103" s="90"/>
-      <c r="E103" s="90"/>
-      <c r="F103" s="90"/>
-      <c r="G103" s="90"/>
-      <c r="H103" s="90"/>
+      <c r="D103" s="91"/>
+      <c r="E103" s="91"/>
+      <c r="F103" s="91"/>
+      <c r="G103" s="91"/>
+      <c r="H103" s="91"/>
     </row>
     <row r="104" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="9"/>
-      <c r="C104" s="90" t="s">
+      <c r="C104" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="D104" s="90"/>
-      <c r="E104" s="90"/>
-      <c r="F104" s="90"/>
-      <c r="G104" s="90"/>
-      <c r="H104" s="90"/>
+      <c r="D104" s="91"/>
+      <c r="E104" s="91"/>
+      <c r="F104" s="91"/>
+      <c r="G104" s="91"/>
+      <c r="H104" s="91"/>
     </row>
     <row r="105" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="9">
         <v>2</v>
       </c>
-      <c r="C105" s="88" t="s">
+      <c r="C105" s="89" t="s">
         <v>104</v>
       </c>
-      <c r="D105" s="88"/>
-      <c r="E105" s="88"/>
-      <c r="F105" s="88"/>
-      <c r="G105" s="88"/>
-      <c r="H105" s="88"/>
+      <c r="D105" s="89"/>
+      <c r="E105" s="89"/>
+      <c r="F105" s="89"/>
+      <c r="G105" s="89"/>
+      <c r="H105" s="89"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B106" s="9">
         <v>3</v>
       </c>
       <c r="C106" s="56" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
@@ -5771,7 +5773,7 @@
         <v>4</v>
       </c>
       <c r="C107" s="75" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
@@ -5779,7 +5781,7 @@
         <v>5</v>
       </c>
       <c r="C108" s="75" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrected U8 part number (had wrong package)
</commit_message>
<xml_diff>
--- a/FPGA1394V3-BOM.xlsx
+++ b/FPGA1394V3-BOM.xlsx
@@ -713,12 +713,6 @@
     <t>Winbond</t>
   </si>
   <si>
-    <t>296-48790-1-ND</t>
-  </si>
-  <si>
-    <t>TXS0101DBVT</t>
-  </si>
-  <si>
     <t>IC, Bidirectional Voltage Translator, TXS0101</t>
   </si>
   <si>
@@ -1494,6 +1488,12 @@
   </si>
   <si>
     <t>XC7Z020-sCLG400t, where s (speed grade) can be 2 or 3 and t (temperature grade) can be C, I or E</t>
+  </si>
+  <si>
+    <t>TXS0101DCK</t>
+  </si>
+  <si>
+    <t>296-22864-1-ND</t>
   </si>
 </sst>
 </file>
@@ -2241,8 +2241,8 @@
   </sheetPr>
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2265,7 +2265,7 @@
     <row r="1" spans="1:13" ht="29.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2280,7 +2280,7 @@
     <row r="2" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2295,7 +2295,7 @@
     <row r="3" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="22">
-        <v>45575</v>
+        <v>45609</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2389,7 +2389,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>175</v>
@@ -2419,7 +2419,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>6</v>
@@ -2462,10 +2462,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>125</v>
@@ -2492,10 +2492,10 @@
         <v>21</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>125</v>
@@ -2524,10 +2524,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D11" s="55" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>125</v>
@@ -2539,11 +2539,11 @@
         <v>2</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K11" s="50"/>
       <c r="L11" s="19"/>
@@ -2558,26 +2558,26 @@
         <v>5</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D12" s="55" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>54</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G12" s="13">
         <v>2</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="K12" s="50"/>
       <c r="L12" s="77">
@@ -2597,26 +2597,26 @@
         <v>13</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G13" s="13">
         <v>2</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K13" s="50"/>
       <c r="L13" s="19">
@@ -2636,26 +2636,26 @@
         <v>2</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>129</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G14" s="13">
         <v>2</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K14" s="50"/>
       <c r="L14" s="77">
@@ -2675,7 +2675,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>136</v>
@@ -2699,7 +2699,7 @@
         <v>134</v>
       </c>
       <c r="K15" s="51" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L15" s="11">
         <v>0.64890000000000003</v>
@@ -2718,7 +2718,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>137</v>
@@ -2742,7 +2742,7 @@
         <v>132</v>
       </c>
       <c r="K16" s="51" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L16" s="11">
         <v>1.2175</v>
@@ -2761,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>150</v>
@@ -2785,7 +2785,7 @@
         <v>152</v>
       </c>
       <c r="K17" s="50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L17" s="11">
         <v>4.8</v>
@@ -2804,7 +2804,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>144</v>
@@ -2828,7 +2828,7 @@
         <v>142</v>
       </c>
       <c r="K18" s="50" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L18" s="19">
         <v>3.2381700000000002</v>
@@ -2847,7 +2847,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>13</v>
@@ -2890,7 +2890,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>12</v>
@@ -2933,26 +2933,26 @@
         <v>2</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>74</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G21" s="13">
         <v>2</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K21" s="50"/>
       <c r="L21" s="87">
@@ -2972,10 +2972,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="83" t="s">
+        <v>412</v>
+      </c>
+      <c r="D22" s="66" t="s">
         <v>414</v>
-      </c>
-      <c r="D22" s="66" t="s">
-        <v>416</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>125</v>
@@ -3002,10 +3002,10 @@
         <v>75</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>176</v>
@@ -3017,11 +3017,11 @@
         <v>2</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K23" s="50"/>
       <c r="L23" s="19"/>
@@ -3036,10 +3036,10 @@
         <v>40</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D24" s="55" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>125</v>
@@ -3051,11 +3051,11 @@
         <v>2</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K24" s="50"/>
       <c r="L24" s="19"/>
@@ -3070,10 +3070,10 @@
         <v>25</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D25" s="55" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>51</v>
@@ -3083,11 +3083,11 @@
         <v>2</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K25" s="50"/>
       <c r="L25" s="19">
@@ -3110,7 +3110,7 @@
         <v>120</v>
       </c>
       <c r="D26" s="55" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>121</v>
@@ -3120,11 +3120,11 @@
         <v>2</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K26" s="50"/>
       <c r="L26" s="19">
@@ -3144,7 +3144,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>18</v>
@@ -3153,19 +3153,19 @@
         <v>54</v>
       </c>
       <c r="F27" s="55" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G27" s="13">
         <v>2</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K27" s="51" t="s">
         <v>90</v>
@@ -3187,7 +3187,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>113</v>
@@ -3285,7 +3285,7 @@
         <v>16</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H30" s="14" t="s">
         <v>15</v>
@@ -3316,26 +3316,26 @@
         <v>1</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D31" s="55" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G31" s="37" t="s">
         <v>11</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K31" s="50"/>
       <c r="L31" s="77">
@@ -3355,13 +3355,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>1</v>
@@ -3398,31 +3398,31 @@
         <v>1</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D33" s="55" t="s">
+        <v>372</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>373</v>
+      </c>
+      <c r="G33" s="13">
+        <v>2</v>
+      </c>
+      <c r="H33" s="51" t="s">
         <v>374</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>375</v>
-      </c>
-      <c r="G33" s="13">
-        <v>2</v>
-      </c>
-      <c r="H33" s="51" t="s">
-        <v>376</v>
       </c>
       <c r="I33" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J33" s="80" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="K33" s="51" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="85"/>
@@ -3436,26 +3436,26 @@
         <v>1</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D34" s="66" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E34" s="66" t="s">
         <v>71</v>
       </c>
       <c r="F34" s="81" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G34" s="37"/>
       <c r="H34" s="80" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I34" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J34" s="66" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="K34" s="80"/>
       <c r="L34" s="82">
@@ -3475,26 +3475,26 @@
         <v>1</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D35" s="66" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E35" s="66" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F35" s="81" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G35" s="37"/>
       <c r="H35" s="80" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I35" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J35" s="66" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K35" s="80"/>
       <c r="L35" s="82">
@@ -3514,31 +3514,31 @@
         <v>1</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D36" s="66" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E36" s="66" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F36" s="81" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G36" s="13">
         <v>2</v>
       </c>
       <c r="H36" s="80" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I36" s="55" t="s">
         <v>52</v>
       </c>
       <c r="J36" s="66" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K36" s="80" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L36" s="82"/>
       <c r="M36" s="85">
@@ -3558,10 +3558,10 @@
         <v>55</v>
       </c>
       <c r="D37" s="55" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E37" s="66" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F37" s="20" t="s">
         <v>135</v>
@@ -3570,7 +3570,7 @@
         <v>11</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
@@ -3592,13 +3592,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D38" s="55" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>135</v>
@@ -3607,7 +3607,7 @@
         <v>11</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
@@ -3632,10 +3632,10 @@
         <v>156</v>
       </c>
       <c r="D39" s="55" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F39" s="20" t="s">
         <v>135</v>
@@ -3644,7 +3644,7 @@
         <v>11</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
@@ -3669,10 +3669,10 @@
         <v>157</v>
       </c>
       <c r="D40" s="55" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F40" s="20" t="s">
         <v>135</v>
@@ -3681,7 +3681,7 @@
         <v>11</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
@@ -3703,13 +3703,13 @@
         <v>2</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D41" s="55" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F41" s="20" t="s">
         <v>135</v>
@@ -3718,7 +3718,7 @@
         <v>11</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
@@ -3740,28 +3740,28 @@
         <v>1</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>51</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G42" s="13">
         <v>2</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I42" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K42" s="51"/>
       <c r="L42" s="19">
@@ -3781,28 +3781,28 @@
         <v>4</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E43" s="64" t="s">
         <v>125</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G43" s="13">
         <v>2</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I43" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K43" s="51"/>
       <c r="L43" s="19">
@@ -3822,7 +3822,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>155</v>
@@ -3951,22 +3951,22 @@
         <v>2</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D47" s="55" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>108</v>
       </c>
       <c r="F47" s="67" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G47" s="68">
         <v>2</v>
       </c>
       <c r="H47" s="69" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I47" s="70"/>
       <c r="J47" s="71"/>
@@ -3990,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>116</v>
@@ -4033,10 +4033,10 @@
         <v>8</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D49" s="55" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E49" s="64" t="s">
         <v>176</v>
@@ -4063,10 +4063,10 @@
         <v>1</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E50" s="64" t="s">
         <v>125</v>
@@ -4093,10 +4093,10 @@
         <v>23</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E51" s="64" t="s">
         <v>125</v>
@@ -4123,10 +4123,10 @@
         <v>3</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E52" s="64" t="s">
         <v>125</v>
@@ -4153,10 +4153,10 @@
         <v>4</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E53" s="64" t="s">
         <v>125</v>
@@ -4183,10 +4183,10 @@
         <v>6</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E54" s="64" t="s">
         <v>125</v>
@@ -4213,10 +4213,10 @@
         <v>10</v>
       </c>
       <c r="C55" s="83" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E55" s="64" t="s">
         <v>125</v>
@@ -4243,10 +4243,10 @@
         <v>5</v>
       </c>
       <c r="C56" s="83" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E56" s="64" t="s">
         <v>125</v>
@@ -4273,7 +4273,7 @@
         <v>0</v>
       </c>
       <c r="C57" s="83" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D57" s="55" t="s">
         <v>0</v>
@@ -4301,10 +4301,10 @@
         <v>4</v>
       </c>
       <c r="C58" s="83" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E58" s="64" t="s">
         <v>125</v>
@@ -4331,10 +4331,10 @@
         <v>2</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E59" s="64" t="s">
         <v>125</v>
@@ -4361,10 +4361,10 @@
         <v>11</v>
       </c>
       <c r="C60" s="63" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E60" s="64" t="s">
         <v>125</v>
@@ -4391,10 +4391,10 @@
         <v>2</v>
       </c>
       <c r="C61" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E61" s="64" t="s">
         <v>125</v>
@@ -4421,10 +4421,10 @@
         <v>2</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E62" s="64" t="s">
         <v>125</v>
@@ -4451,10 +4451,10 @@
         <v>11</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E63" s="64" t="s">
         <v>125</v>
@@ -4481,10 +4481,10 @@
         <v>1</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E64" s="64" t="s">
         <v>125</v>
@@ -4511,10 +4511,10 @@
         <v>1</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D65" s="66" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E65" s="64" t="s">
         <v>125</v>
@@ -4541,10 +4541,10 @@
         <v>2</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D66" s="66" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E66" s="64" t="s">
         <v>125</v>
@@ -4571,10 +4571,10 @@
         <v>1</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E67" s="64" t="s">
         <v>125</v>
@@ -4584,11 +4584,11 @@
         <v>2</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I67" s="10"/>
       <c r="J67" s="10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K67" s="50"/>
       <c r="L67" s="19">
@@ -4608,10 +4608,10 @@
         <v>7</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E68" s="64" t="s">
         <v>125</v>
@@ -4621,11 +4621,11 @@
         <v>2</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I68" s="10"/>
       <c r="J68" s="10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K68" s="50"/>
       <c r="L68" s="19">
@@ -4645,10 +4645,10 @@
         <v>1</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E69" s="64" t="s">
         <v>125</v>
@@ -4658,11 +4658,11 @@
         <v>2</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I69" s="10"/>
       <c r="J69" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K69" s="51"/>
       <c r="L69" s="19">
@@ -4682,10 +4682,10 @@
         <v>2</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E70" s="64" t="s">
         <v>125</v>
@@ -4695,11 +4695,11 @@
         <v>2</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I70" s="10"/>
       <c r="J70" s="10" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K70" s="50"/>
       <c r="L70" s="19">
@@ -4719,10 +4719,10 @@
         <v>1</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D71" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E71" s="64" t="s">
         <v>125</v>
@@ -4732,11 +4732,11 @@
         <v>2</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I71" s="10"/>
       <c r="J71" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K71" s="50"/>
       <c r="L71" s="77">
@@ -4756,7 +4756,7 @@
         <v>8</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D72" s="20" t="s">
         <v>97</v>
@@ -4799,10 +4799,10 @@
         <v>2</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E73" s="21" t="s">
         <v>69</v>
@@ -4812,13 +4812,13 @@
         <v>2</v>
       </c>
       <c r="H73" s="10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I73" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="K73" s="51"/>
       <c r="L73" s="19">
@@ -4927,7 +4927,7 @@
         <v>50</v>
       </c>
       <c r="D76" s="55" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>159</v>
@@ -4939,13 +4939,13 @@
         <v>5</v>
       </c>
       <c r="H76" s="66" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I76" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J76" s="62" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K76" s="62"/>
       <c r="L76" s="19">
@@ -4968,7 +4968,7 @@
         <v>160</v>
       </c>
       <c r="D77" s="55" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>161</v>
@@ -5009,7 +5009,7 @@
         <v>122</v>
       </c>
       <c r="D78" s="55" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>162</v>
@@ -5021,11 +5021,11 @@
         <v>11</v>
       </c>
       <c r="H78" s="51" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I78" s="10"/>
       <c r="J78" s="51" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="K78" s="62"/>
       <c r="L78" s="77">
@@ -5173,7 +5173,7 @@
         <v>165</v>
       </c>
       <c r="D82" s="55" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>108</v>
@@ -5185,21 +5185,21 @@
         <v>2</v>
       </c>
       <c r="H82" s="14" t="s">
-        <v>201</v>
+        <v>418</v>
       </c>
       <c r="I82" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>200</v>
+        <v>419</v>
       </c>
       <c r="K82" s="62"/>
       <c r="L82" s="19">
-        <v>0.86060000000000003</v>
+        <v>0.27329999999999999</v>
       </c>
       <c r="M82" s="85">
         <f t="shared" si="5"/>
-        <v>0.86060000000000003</v>
+        <v>0.27329999999999999</v>
       </c>
     </row>
     <row r="83" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -5214,25 +5214,25 @@
         <v>166</v>
       </c>
       <c r="D83" s="55" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>108</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G83" s="13">
         <v>2</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I83" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K83" s="62"/>
       <c r="L83" s="77">
@@ -5252,7 +5252,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D84" s="10" t="s">
         <v>196</v>
@@ -5287,7 +5287,7 @@
         <v>2</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D85" s="20" t="s">
         <v>28</v>
@@ -5330,7 +5330,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D86" s="10" t="s">
         <v>126</v>
@@ -5373,7 +5373,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D87" s="10" t="s">
         <v>197</v>
@@ -5414,10 +5414,10 @@
         <v>1</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>172</v>
@@ -5458,7 +5458,7 @@
         <v>168</v>
       </c>
       <c r="D89" s="55" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>174</v>
@@ -5470,11 +5470,11 @@
         <v>1</v>
       </c>
       <c r="H89" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I89" s="10"/>
       <c r="J89" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K89" s="62"/>
       <c r="L89" s="77">
@@ -5536,25 +5536,25 @@
         <v>171</v>
       </c>
       <c r="D91" s="66" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E91" s="15" t="s">
         <v>123</v>
       </c>
       <c r="F91" s="66" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G91" s="13">
         <v>2</v>
       </c>
       <c r="H91" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I91" s="10" t="s">
         <v>52</v>
       </c>
       <c r="J91" s="10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K91" s="60" t="s">
         <v>180</v>
@@ -5579,23 +5579,23 @@
         <v>173</v>
       </c>
       <c r="D92" s="66" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>123</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G92" s="13">
         <v>2</v>
       </c>
       <c r="H92" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I92" s="10"/>
       <c r="J92" s="55" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K92" s="50"/>
       <c r="L92" s="77">
@@ -5616,7 +5616,7 @@
       </c>
       <c r="C93" s="30"/>
       <c r="D93" s="73" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E93" s="32"/>
       <c r="F93" s="31"/>
@@ -5643,7 +5643,7 @@
       </c>
       <c r="M94" s="36">
         <f>SUM(M7:M93)</f>
-        <v>367.65541758620685</v>
+        <v>367.06811758620688</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -5675,7 +5675,7 @@
         <v>94</v>
       </c>
       <c r="C99" s="76" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D99" s="72"/>
       <c r="E99" s="72"/>
@@ -5765,7 +5765,7 @@
         <v>3</v>
       </c>
       <c r="C106" s="56" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
@@ -5773,7 +5773,7 @@
         <v>4</v>
       </c>
       <c r="C107" s="75" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
@@ -5781,7 +5781,7 @@
         <v>5</v>
       </c>
       <c r="C108" s="75" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>